<commit_message>
re-arranges columns in excel file per Paul. Working on formatting
</commit_message>
<xml_diff>
--- a/OWGR.xlsx
+++ b/OWGR.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="127">
+  <si>
+    <t>RANK</t>
+  </si>
   <si>
     <t>Player Name</t>
   </si>
@@ -23,9 +26,6 @@
     <t>Headshot</t>
   </si>
   <si>
-    <t>Rank</t>
-  </si>
-  <si>
     <t>Johnson, Dustin</t>
   </si>
   <si>
@@ -47,24 +47,24 @@
     <t>Fowler, Rickie</t>
   </si>
   <si>
+    <t>Day, Jason</t>
+  </si>
+  <si>
+    <t>Koepka, Brooks</t>
+  </si>
+  <si>
     <t>McIlroy, Rory</t>
   </si>
   <si>
-    <t>Koepka, Brooks</t>
-  </si>
-  <si>
-    <t>Day, Jason</t>
-  </si>
-  <si>
     <t>Garcia, Sergio</t>
   </si>
   <si>
+    <t>Stenson, Henrik</t>
+  </si>
+  <si>
     <t>Fleetwood, Tommy</t>
   </si>
   <si>
-    <t>Stenson, Henrik</t>
-  </si>
-  <si>
     <t>Leishman, Marc</t>
   </si>
   <si>
@@ -83,12 +83,12 @@
     <t>Perez, Pat</t>
   </si>
   <si>
+    <t>Cabrera Bello, Rafael</t>
+  </si>
+  <si>
     <t>Harman, Brian</t>
   </si>
   <si>
-    <t>Cabrera Bello, Rafael</t>
-  </si>
-  <si>
     <t>Molinari, Francesco</t>
   </si>
   <si>
@@ -128,72 +128,75 @@
     <t>Chappell, Kevin</t>
   </si>
   <si>
+    <t>Mickelson, Phil</t>
+  </si>
+  <si>
     <t>Steele, Brendan</t>
   </si>
   <si>
+    <t>Aphibarnrat, Kiradech</t>
+  </si>
+  <si>
     <t>Pieters, Thomas</t>
   </si>
   <si>
+    <t>Cantlay, Patrick</t>
+  </si>
+  <si>
     <t>Kodaira, Satoshi</t>
   </si>
   <si>
-    <t>Cantlay, Patrick</t>
-  </si>
-  <si>
     <t>Finau, Tony</t>
   </si>
   <si>
+    <t>Simpson, Webb</t>
+  </si>
+  <si>
+    <t>Reavie, Chez</t>
+  </si>
+  <si>
     <t>Schwartzel, Charl</t>
   </si>
   <si>
-    <t>Mickelson, Phil</t>
-  </si>
-  <si>
     <t>Vegas, Jhonattan</t>
   </si>
   <si>
+    <t>Ikeda, Yuta</t>
+  </si>
+  <si>
+    <t>Dufner, Jason</t>
+  </si>
+  <si>
+    <t>Kim, Siwoo</t>
+  </si>
+  <si>
+    <t>Frittelli, Dylan</t>
+  </si>
+  <si>
+    <t>Wiesberger, Bernd</t>
+  </si>
+  <si>
     <t>Scott, Adam</t>
   </si>
   <si>
-    <t>Ikeda, Yuta</t>
-  </si>
-  <si>
-    <t>Kim, Siwoo</t>
-  </si>
-  <si>
-    <t>Simpson, Webb</t>
-  </si>
-  <si>
-    <t>Frittelli, Dylan</t>
-  </si>
-  <si>
-    <t>Dufner, Jason</t>
-  </si>
-  <si>
-    <t>Wiesberger, Bernd</t>
+    <t>Miyazato, Yusaku</t>
   </si>
   <si>
     <t>Stanley, Kyle</t>
   </si>
   <si>
-    <t>Miyazato, Yusaku</t>
+    <t>Henley, Russell</t>
   </si>
   <si>
     <t>Johnson, Zach</t>
   </si>
   <si>
-    <t>Aphibarnrat, Kiradech</t>
+    <t>Kizzire, Patton</t>
   </si>
   <si>
     <t>Hadwin, Adam</t>
   </si>
   <si>
-    <t>Kizzire, Patton</t>
-  </si>
-  <si>
-    <t>Henley, Russell</t>
-  </si>
-  <si>
     <t>Smith, Cameron</t>
   </si>
   <si>
@@ -206,9 +209,6 @@
     <t>Hahn, James</t>
   </si>
   <si>
-    <t>Reavie, Chez</t>
-  </si>
-  <si>
     <t>Levy, Alexander</t>
   </si>
   <si>
@@ -218,15 +218,15 @@
     <t>Bradley, Keegan</t>
   </si>
   <si>
+    <t>Suri, Julian</t>
+  </si>
+  <si>
+    <t>Snedeker, Brandt</t>
+  </si>
+  <si>
     <t>Haas, Bill</t>
   </si>
   <si>
-    <t>Suri, Julian</t>
-  </si>
-  <si>
-    <t>Snedeker, Brandt</t>
-  </si>
-  <si>
     <t>Hadley, Chesson</t>
   </si>
   <si>
@@ -236,10 +236,13 @@
     <t>Moore, Ryan</t>
   </si>
   <si>
+    <t>Sharma, Shubhankar</t>
+  </si>
+  <si>
     <t>Tanihara, Hideto</t>
   </si>
   <si>
-    <t>Sharma, Shubhankar</t>
+    <t>Potter Jr, Ted</t>
   </si>
   <si>
     <t>Westwood, Lee</t>
@@ -254,42 +257,42 @@
     <t>Lahiri, Anirban</t>
   </si>
   <si>
+    <t>Kaymer, Martin</t>
+  </si>
+  <si>
     <t>Schniederjans, Ollie</t>
   </si>
   <si>
+    <t>Dunne, Paul</t>
+  </si>
+  <si>
     <t>Grillo, Emiliano</t>
   </si>
   <si>
-    <t>Kaymer, Martin</t>
-  </si>
-  <si>
-    <t>Dunne, Paul</t>
+    <t>Walker, Jimmy</t>
+  </si>
+  <si>
+    <t>Paisley, Chris</t>
   </si>
   <si>
     <t>Holmes, J.B.</t>
   </si>
   <si>
-    <t>Paisley, Chris</t>
-  </si>
-  <si>
     <t>Knox, Russell</t>
   </si>
   <si>
-    <t>Walker, Jimmy</t>
+    <t>Olesen, Thorbjorn</t>
+  </si>
+  <si>
+    <t>Kim, Chan</t>
+  </si>
+  <si>
+    <t>Han, Seungsu</t>
   </si>
   <si>
     <t>DeChambeau, Bryson</t>
   </si>
   <si>
-    <t>Kim, Chan</t>
-  </si>
-  <si>
-    <t>Han, Seungsu</t>
-  </si>
-  <si>
-    <t>Olesen, Thorbjorn</t>
-  </si>
-  <si>
     <t>Luiten, Joost</t>
   </si>
   <si>
@@ -305,24 +308,27 @@
     <t>Imahira, Shugo</t>
   </si>
   <si>
+    <t>Na, Kevin</t>
+  </si>
+  <si>
     <t>Dubuisson, Victor</t>
   </si>
   <si>
     <t>Fox, Ryan</t>
   </si>
   <si>
+    <t>Palmer, Ryan</t>
+  </si>
+  <si>
     <t>Swafford, Hudson</t>
   </si>
   <si>
-    <t>Na, Kevin</t>
+    <t>Zanotti, Fabrizio</t>
   </si>
   <si>
     <t>Im, Sungjae</t>
   </si>
   <si>
-    <t>Palmer, Ryan</t>
-  </si>
-  <si>
     <t>L Smith, Jordan</t>
   </si>
   <si>
@@ -339,9 +345,6 @@
   </si>
   <si>
     <t>Fitzpatrick, Mathew</t>
-  </si>
-  <si>
-    <t>Flettwood, Tommy</t>
   </si>
   <si>
     <t>Furyk, Jim</t>
@@ -400,13 +403,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -448,8 +454,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="justify"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -461,12 +470,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table1" headerRowCount="1" id="1" name="Table1" ref="B3:D126">
-  <autoFilter ref="B3:D126"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table1" headerRowCount="1" id="1" name="Table1" ref="B3:D127">
+  <autoFilter ref="B3:D127"/>
   <tableColumns count="3">
-    <tableColumn id="2" name="Player Name"/>
-    <tableColumn id="3" name="Headshot"/>
-    <tableColumn id="4" name="Rank"/>
+    <tableColumn id="2" name="RANK"/>
+    <tableColumn id="3" name="Player Name"/>
+    <tableColumn id="4" name="Headshot"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="0"/>
 </table>
@@ -761,7 +770,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:D126"/>
+  <dimension ref="B3:D127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -784,1111 +793,1120 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="n"/>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2" t="n"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="n"/>
-      <c r="D5" t="n">
-        <v>2</v>
-      </c>
+      <c r="D5" s="2" t="n"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="n"/>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
+      <c r="D6" s="2" t="n"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="n"/>
-      <c r="D7" t="n">
-        <v>4</v>
-      </c>
+      <c r="D7" s="2" t="n"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="n"/>
-      <c r="D8" t="n">
-        <v>5</v>
-      </c>
+      <c r="D8" s="2" t="n"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="n"/>
-      <c r="D9" t="n">
-        <v>6</v>
-      </c>
+      <c r="D9" s="2" t="n"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="n"/>
-      <c r="D10" t="n">
-        <v>7</v>
-      </c>
+      <c r="D10" s="2" t="n"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="n"/>
-      <c r="D11" t="n">
-        <v>8</v>
-      </c>
+      <c r="D11" s="2" t="n"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="n"/>
-      <c r="D12" t="n">
-        <v>9</v>
-      </c>
+      <c r="D12" s="2" t="n"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1" t="n"/>
-      <c r="D13" t="n">
-        <v>10</v>
-      </c>
+      <c r="D13" s="2" t="n"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="n"/>
-      <c r="D14" t="n">
-        <v>11</v>
-      </c>
+      <c r="D14" s="2" t="n"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="2" t="n"/>
-      <c r="D15" t="n">
-        <v>12</v>
-      </c>
+      <c r="D15" s="2" t="n"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="1" t="n"/>
-      <c r="D16" t="n">
-        <v>13</v>
-      </c>
+      <c r="D16" s="2" t="n"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="n"/>
-      <c r="D17" t="n">
-        <v>14</v>
-      </c>
+      <c r="D17" s="2" t="n"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="n"/>
-      <c r="D18" t="n">
-        <v>15</v>
-      </c>
+      <c r="D18" s="3" t="n"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="1" t="n"/>
-      <c r="D19" t="n">
-        <v>16</v>
-      </c>
+      <c r="D19" s="2" t="n"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="1" t="n"/>
-      <c r="D20" t="n">
-        <v>17</v>
-      </c>
+      <c r="D20" s="2" t="n"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="1" t="n"/>
-      <c r="D21" t="n">
-        <v>18</v>
-      </c>
+      <c r="D21" s="2" t="n"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="1" t="n"/>
-      <c r="D22" t="n">
-        <v>19</v>
-      </c>
+      <c r="D22" s="2" t="n"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="2" t="n"/>
-      <c r="D23" t="n">
-        <v>20</v>
-      </c>
+      <c r="D23" s="3" t="n"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="2" t="n"/>
-      <c r="D24" t="n">
-        <v>21</v>
-      </c>
+      <c r="D24" s="3" t="n"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="1" t="n"/>
-      <c r="D25" t="n">
-        <v>22</v>
-      </c>
+      <c r="D25" s="2" t="n"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="2" t="n"/>
-      <c r="D26" t="n">
-        <v>23</v>
-      </c>
+      <c r="D26" s="3" t="n"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="1" t="n"/>
-      <c r="D27" t="n">
-        <v>24</v>
-      </c>
+      <c r="D27" s="2" t="n"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="2" t="n"/>
-      <c r="D28" t="n">
-        <v>25</v>
-      </c>
+      <c r="D28" s="3" t="n"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="1" t="n"/>
-      <c r="D29" t="n">
-        <v>26</v>
-      </c>
+      <c r="D29" s="2" t="n"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="C30" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="1" t="n"/>
-      <c r="D30" t="n">
-        <v>27</v>
-      </c>
+      <c r="D30" s="2" t="n"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="C31" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="1" t="n"/>
-      <c r="D31" t="n">
-        <v>28</v>
-      </c>
+      <c r="D31" s="2" t="n"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="1" t="n"/>
-      <c r="D32" t="n">
-        <v>29</v>
-      </c>
+      <c r="D32" s="2" t="n"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="2" t="n"/>
-      <c r="D33" t="n">
-        <v>30</v>
-      </c>
+      <c r="D33" s="3" t="n"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="C34" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="1" t="n"/>
-      <c r="D34" t="n">
-        <v>31</v>
-      </c>
+      <c r="D34" s="2" t="n"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="C35" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="1" t="n"/>
-      <c r="D35" t="n">
-        <v>32</v>
-      </c>
+      <c r="D35" s="2" t="n"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="C36" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="2" t="n"/>
-      <c r="D36" t="n">
-        <v>33</v>
-      </c>
+      <c r="D36" s="3" t="n"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="C37" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="1" t="n"/>
-      <c r="D37" t="n">
-        <v>34</v>
-      </c>
+      <c r="D37" s="2" t="n"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="C38" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="1" t="n"/>
-      <c r="D38" t="n">
-        <v>35</v>
-      </c>
+      <c r="D38" s="2" t="n"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="1" t="n"/>
-      <c r="D39" t="n">
-        <v>36</v>
-      </c>
+      <c r="D39" s="2" t="n"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="C40" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="2" t="n"/>
-      <c r="D40" t="n">
-        <v>37</v>
-      </c>
+      <c r="D40" s="3" t="n"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="C41" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="2" t="n"/>
-      <c r="D41" t="n">
-        <v>38</v>
-      </c>
+      <c r="D41" s="2" t="n"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="C42" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="2" t="n"/>
-      <c r="D42" t="n">
-        <v>39</v>
-      </c>
+      <c r="D42" s="3" t="n"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="C43" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="1" t="n"/>
-      <c r="D43" t="n">
-        <v>40</v>
-      </c>
+      <c r="D43" s="3" t="n"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="C44" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="1" t="n"/>
-      <c r="D44" t="n">
-        <v>41</v>
-      </c>
+      <c r="D44" s="3" t="n"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="C45" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="1" t="n"/>
-      <c r="D45" t="n">
-        <v>42</v>
-      </c>
+      <c r="D45" s="2" t="n"/>
     </row>
     <row r="46" spans="1:4">
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="C46" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="2" t="n"/>
-      <c r="D46" t="n">
-        <v>43</v>
-      </c>
+      <c r="D46" s="3" t="n"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="C47" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="1" t="n"/>
-      <c r="D47" t="n">
-        <v>44</v>
-      </c>
+      <c r="D47" s="2" t="n"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="C48" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="2" t="n"/>
-      <c r="D48" t="n">
-        <v>45</v>
-      </c>
+      <c r="D48" s="2" t="n"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="C49" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="1" t="n"/>
-      <c r="D49" t="n">
-        <v>46</v>
-      </c>
+      <c r="D49" s="2" t="n"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="C50" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="2" t="n"/>
-      <c r="D50" t="n">
-        <v>47</v>
-      </c>
+      <c r="D50" s="2" t="n"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="B51" t="s">
+      <c r="B51" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="C51" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="1" t="n"/>
-      <c r="D51" t="n">
-        <v>48</v>
-      </c>
+      <c r="D51" s="3" t="n"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="B52" t="s">
+      <c r="B52" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="C52" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="1" t="n"/>
-      <c r="D52" t="n">
-        <v>49</v>
-      </c>
+      <c r="D52" s="3" t="n"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="C53" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="2" t="n"/>
-      <c r="D53" t="n">
-        <v>50</v>
-      </c>
+      <c r="D53" s="2" t="n"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="B54" t="s">
+      <c r="B54" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="C54" t="s">
         <v>53</v>
       </c>
-      <c r="C54" s="2" t="n"/>
-      <c r="D54" t="n">
-        <v>51</v>
-      </c>
+      <c r="D54" s="3" t="n"/>
     </row>
     <row r="55" spans="1:4">
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="C55" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="1" t="n"/>
-      <c r="D55" t="n">
-        <v>52</v>
-      </c>
+      <c r="D55" s="3" t="n"/>
     </row>
     <row r="56" spans="1:4">
-      <c r="B56" t="s">
+      <c r="B56" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="C56" t="s">
         <v>55</v>
       </c>
-      <c r="C56" s="2" t="n"/>
-      <c r="D56" t="n">
-        <v>53</v>
-      </c>
+      <c r="D56" s="3" t="n"/>
     </row>
     <row r="57" spans="1:4">
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="C57" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="1" t="n"/>
-      <c r="D57" t="n">
-        <v>54</v>
-      </c>
+      <c r="D57" s="3" t="n"/>
     </row>
     <row r="58" spans="1:4">
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="C58" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="2" t="n"/>
-      <c r="D58" t="n">
-        <v>55</v>
-      </c>
+      <c r="D58" s="2" t="n"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="B59" t="s">
+      <c r="B59" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="C59" t="s">
         <v>58</v>
       </c>
-      <c r="C59" s="2" t="n"/>
-      <c r="D59" t="n">
-        <v>56</v>
-      </c>
+      <c r="D59" s="3" t="n"/>
     </row>
     <row r="60" spans="1:4">
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="C60" t="s">
         <v>59</v>
       </c>
-      <c r="C60" s="2" t="n"/>
-      <c r="D60" t="n">
-        <v>57</v>
-      </c>
+      <c r="D60" s="2" t="n"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="B61" t="s">
+      <c r="B61" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="C61" t="s">
         <v>60</v>
       </c>
-      <c r="C61" s="2" t="n"/>
-      <c r="D61" t="n">
-        <v>58</v>
-      </c>
+      <c r="D61" s="3" t="n"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="C62" t="s">
         <v>61</v>
       </c>
-      <c r="C62" s="2" t="n"/>
-      <c r="D62" t="n">
-        <v>59</v>
-      </c>
+      <c r="D62" s="3" t="n"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C63" t="s">
         <v>62</v>
       </c>
-      <c r="C63" s="2" t="n"/>
-      <c r="D63" t="n">
-        <v>60</v>
-      </c>
+      <c r="D63" s="3" t="n"/>
     </row>
     <row r="64" spans="1:4">
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="C64" t="s">
         <v>63</v>
       </c>
-      <c r="C64" s="2" t="n"/>
-      <c r="D64" t="n">
-        <v>61</v>
-      </c>
+      <c r="D64" s="3" t="n"/>
     </row>
     <row r="65" spans="1:4">
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="C65" t="s">
         <v>64</v>
       </c>
-      <c r="C65" s="2" t="n"/>
-      <c r="D65" t="n">
-        <v>62</v>
-      </c>
+      <c r="D65" s="3" t="n"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="C66" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="1" t="n"/>
-      <c r="D66" t="n">
-        <v>63</v>
-      </c>
+      <c r="D66" s="2" t="n"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="B67" t="s">
+      <c r="B67" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="C67" t="s">
         <v>66</v>
       </c>
-      <c r="C67" s="2" t="n"/>
-      <c r="D67" t="n">
-        <v>64</v>
-      </c>
+      <c r="D67" s="3" t="n"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="B68" t="s">
+      <c r="B68" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="C68" t="s">
         <v>67</v>
       </c>
-      <c r="C68" s="1" t="n"/>
-      <c r="D68" t="n">
-        <v>65</v>
-      </c>
+      <c r="D68" s="3" t="n"/>
     </row>
     <row r="69" spans="1:4">
-      <c r="B69" t="s">
+      <c r="B69" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="C69" t="s">
         <v>68</v>
       </c>
-      <c r="C69" s="2" t="n"/>
-      <c r="D69" t="n">
-        <v>66</v>
-      </c>
+      <c r="D69" s="2" t="n"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="B70" t="s">
+      <c r="B70" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="C70" t="s">
         <v>69</v>
       </c>
-      <c r="C70" s="1" t="n"/>
-      <c r="D70" t="n">
-        <v>67</v>
-      </c>
+      <c r="D70" s="2" t="n"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="B71" t="s">
+      <c r="B71" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="C71" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="2" t="n"/>
-      <c r="D71" t="n">
-        <v>68</v>
-      </c>
+      <c r="D71" s="3" t="n"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="B72" t="s">
+      <c r="B72" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="C72" t="s">
         <v>71</v>
       </c>
-      <c r="C72" s="1" t="n"/>
-      <c r="D72" t="n">
-        <v>69</v>
-      </c>
+      <c r="D72" s="2" t="n"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="B73" t="s">
+      <c r="B73" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="C73" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="1" t="n"/>
-      <c r="D73" t="n">
-        <v>70</v>
-      </c>
+      <c r="D73" s="2" t="n"/>
     </row>
     <row r="74" spans="1:4">
-      <c r="B74" t="s">
+      <c r="B74" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="C74" t="s">
         <v>73</v>
       </c>
-      <c r="C74" s="1" t="n"/>
-      <c r="D74" t="n">
-        <v>71</v>
-      </c>
+      <c r="D74" s="3" t="n"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="B75" t="s">
+      <c r="B75" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="C75" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="2" t="n"/>
-      <c r="D75" t="n">
-        <v>72</v>
-      </c>
+      <c r="D75" s="2" t="n"/>
     </row>
     <row r="76" spans="1:4">
-      <c r="B76" t="s">
+      <c r="B76" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="C76" t="s">
         <v>75</v>
       </c>
-      <c r="C76" s="2" t="n"/>
-      <c r="D76" t="n">
-        <v>73</v>
-      </c>
+      <c r="D76" s="3" t="n"/>
     </row>
     <row r="77" spans="1:4">
-      <c r="B77" t="s">
+      <c r="B77" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="C77" t="s">
         <v>76</v>
       </c>
-      <c r="C77" s="1" t="n"/>
-      <c r="D77" t="n">
-        <v>74</v>
-      </c>
+      <c r="D77" s="2" t="n"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="B78" t="s">
+      <c r="B78" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="C78" t="s">
         <v>77</v>
       </c>
-      <c r="C78" s="2" t="n"/>
-      <c r="D78" t="n">
-        <v>75</v>
-      </c>
+      <c r="D78" s="2" t="n"/>
     </row>
     <row r="79" spans="1:4">
-      <c r="B79" t="s">
+      <c r="B79" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="C79" t="s">
         <v>78</v>
       </c>
-      <c r="C79" s="2" t="n"/>
-      <c r="D79" t="n">
-        <v>76</v>
-      </c>
+      <c r="D79" s="3" t="n"/>
     </row>
     <row r="80" spans="1:4">
-      <c r="B80" t="s">
+      <c r="B80" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="C80" t="s">
         <v>79</v>
       </c>
-      <c r="C80" s="2" t="n"/>
-      <c r="D80" t="n">
-        <v>77</v>
-      </c>
+      <c r="D80" s="3" t="n"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="B81" t="s">
+      <c r="B81" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="C81" t="s">
         <v>80</v>
       </c>
-      <c r="C81" s="1" t="n"/>
-      <c r="D81" t="n">
-        <v>78</v>
-      </c>
+      <c r="D81" s="2" t="n"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="B82" t="s">
+      <c r="B82" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="C82" t="s">
         <v>81</v>
       </c>
-      <c r="C82" s="1" t="n"/>
-      <c r="D82" t="n">
-        <v>79</v>
-      </c>
+      <c r="D82" s="3" t="n"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="B83" t="s">
+      <c r="B83" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="C83" t="s">
         <v>82</v>
       </c>
-      <c r="C83" s="2" t="n"/>
-      <c r="D83" t="n">
-        <v>80</v>
-      </c>
+      <c r="D83" s="3" t="n"/>
     </row>
     <row r="84" spans="1:4">
-      <c r="B84" t="s">
+      <c r="B84" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="C84" t="s">
         <v>83</v>
       </c>
-      <c r="C84" s="1" t="n"/>
-      <c r="D84" t="n">
-        <v>81</v>
-      </c>
+      <c r="D84" s="2" t="n"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="B85" t="s">
+      <c r="B85" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="C85" t="s">
         <v>84</v>
       </c>
-      <c r="C85" s="2" t="n"/>
-      <c r="D85" t="n">
-        <v>82</v>
-      </c>
+      <c r="D85" s="2" t="n"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="B86" t="s">
+      <c r="B86" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="C86" t="s">
         <v>85</v>
       </c>
-      <c r="C86" s="1" t="n"/>
-      <c r="D86" t="n">
-        <v>83</v>
-      </c>
+      <c r="D86" s="3" t="n"/>
     </row>
     <row r="87" spans="1:4">
-      <c r="B87" t="s">
+      <c r="B87" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="C87" t="s">
         <v>86</v>
       </c>
-      <c r="C87" s="1" t="n"/>
-      <c r="D87" t="n">
-        <v>84</v>
-      </c>
+      <c r="D87" s="2" t="n"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="B88" t="s">
+      <c r="B88" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="C88" t="s">
         <v>87</v>
       </c>
-      <c r="C88" s="2" t="n"/>
-      <c r="D88" t="n">
-        <v>85</v>
-      </c>
+      <c r="D88" s="2" t="n"/>
     </row>
     <row r="89" spans="1:4">
-      <c r="B89" t="s">
+      <c r="B89" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="C89" t="s">
         <v>88</v>
       </c>
-      <c r="C89" s="2" t="n"/>
-      <c r="D89" t="n">
-        <v>86</v>
-      </c>
+      <c r="D89" s="3" t="n"/>
     </row>
     <row r="90" spans="1:4">
-      <c r="B90" t="s">
+      <c r="B90" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="C90" t="s">
         <v>89</v>
       </c>
-      <c r="C90" s="2" t="n"/>
-      <c r="D90" t="n">
-        <v>87</v>
-      </c>
+      <c r="D90" s="3" t="n"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="B91" t="s">
+      <c r="B91" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="C91" t="s">
         <v>90</v>
       </c>
-      <c r="C91" s="2" t="n"/>
-      <c r="D91" t="n">
-        <v>88</v>
-      </c>
+      <c r="D91" s="3" t="n"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="B92" t="s">
+      <c r="B92" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="C92" t="s">
         <v>91</v>
       </c>
-      <c r="C92" s="1" t="n"/>
-      <c r="D92" t="n">
-        <v>89</v>
-      </c>
+      <c r="D92" s="3" t="n"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="B93" t="s">
+      <c r="B93" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="C93" t="s">
         <v>92</v>
       </c>
-      <c r="C93" s="2" t="n"/>
-      <c r="D93" t="n">
-        <v>90</v>
-      </c>
+      <c r="D93" s="2" t="n"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="B94" t="s">
+      <c r="B94" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="C94" t="s">
         <v>93</v>
       </c>
-      <c r="C94" s="2" t="n"/>
-      <c r="D94" t="n">
-        <v>91</v>
-      </c>
+      <c r="D94" s="3" t="n"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="B95" t="s">
+      <c r="B95" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="C95" t="s">
         <v>94</v>
       </c>
-      <c r="C95" s="1" t="n"/>
-      <c r="D95" t="n">
-        <v>92</v>
-      </c>
+      <c r="D95" s="3" t="n"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="B96" t="s">
+      <c r="B96" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="C96" t="s">
         <v>95</v>
       </c>
-      <c r="C96" s="2" t="n"/>
-      <c r="D96" t="n">
-        <v>93</v>
-      </c>
+      <c r="D96" s="2" t="n"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="B97" t="s">
+      <c r="B97" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="C97" t="s">
         <v>96</v>
       </c>
-      <c r="C97" s="2" t="n"/>
-      <c r="D97" t="n">
-        <v>94</v>
-      </c>
+      <c r="D97" s="3" t="n"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="B98" t="s">
+      <c r="B98" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="C98" t="s">
         <v>97</v>
       </c>
-      <c r="C98" s="2" t="n"/>
-      <c r="D98" t="n">
-        <v>95</v>
-      </c>
+      <c r="D98" s="2" t="n"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="B99" t="s">
+      <c r="B99" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C99" t="s">
         <v>98</v>
       </c>
-      <c r="C99" s="2" t="n"/>
-      <c r="D99" t="n">
-        <v>96</v>
-      </c>
+      <c r="D99" s="3" t="n"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="B100" t="s">
+      <c r="B100" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="C100" t="s">
         <v>99</v>
       </c>
-      <c r="C100" s="1" t="n"/>
-      <c r="D100" t="n">
-        <v>97</v>
-      </c>
+      <c r="D100" s="3" t="n"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="B101" t="s">
+      <c r="B101" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="C101" t="s">
         <v>100</v>
       </c>
-      <c r="C101" s="2" t="n"/>
-      <c r="D101" t="n">
-        <v>98</v>
-      </c>
+      <c r="D101" s="3" t="n"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="B102" t="s">
-        <v>101</v>
-      </c>
-      <c r="C102" s="2" t="n"/>
-      <c r="D102" t="n">
+      <c r="B102" s="1" t="n">
         <v>99</v>
       </c>
+      <c r="C102" t="s">
+        <v>101</v>
+      </c>
+      <c r="D102" s="3" t="n"/>
     </row>
     <row r="103" spans="1:4">
-      <c r="B103" t="s">
+      <c r="B103" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="C103" t="s">
         <v>102</v>
       </c>
-      <c r="C103" s="2" t="n"/>
-      <c r="D103" t="n">
-        <v>100</v>
-      </c>
+      <c r="D103" s="3" t="n"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="B104" t="s">
+      <c r="B104" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C104" t="s">
         <v>103</v>
       </c>
-      <c r="C104" s="1" t="n"/>
-      <c r="D104" t="n">
-        <v>101</v>
-      </c>
+      <c r="D104" s="3" t="n"/>
     </row>
     <row r="105" spans="1:4">
-      <c r="B105" t="s">
+      <c r="B105" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C105" t="s">
         <v>104</v>
       </c>
-      <c r="C105" s="1" t="n"/>
-      <c r="D105" t="n">
-        <v>101</v>
-      </c>
+      <c r="D105" s="3" t="n"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="B106" t="s">
+      <c r="B106" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C106" t="s">
         <v>105</v>
       </c>
-      <c r="C106" s="1" t="n"/>
-      <c r="D106" t="n">
-        <v>101</v>
-      </c>
+      <c r="D106" s="2" t="n"/>
     </row>
     <row r="107" spans="1:4">
-      <c r="B107" t="s">
+      <c r="B107" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C107" t="s">
         <v>106</v>
       </c>
-      <c r="C107" s="1" t="n"/>
-      <c r="D107" t="n">
-        <v>101</v>
-      </c>
+      <c r="D107" s="2" t="n"/>
     </row>
     <row r="108" spans="1:4">
-      <c r="B108" t="s">
+      <c r="B108" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C108" t="s">
         <v>107</v>
       </c>
-      <c r="C108" s="1" t="n"/>
-      <c r="D108" t="n">
-        <v>101</v>
-      </c>
+      <c r="D108" s="2" t="n"/>
     </row>
     <row r="109" spans="1:4">
-      <c r="B109" t="s">
+      <c r="B109" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C109" t="s">
         <v>108</v>
       </c>
-      <c r="C109" s="1" t="n"/>
-      <c r="D109" t="n">
-        <v>101</v>
-      </c>
+      <c r="D109" s="2" t="n"/>
     </row>
     <row r="110" spans="1:4">
-      <c r="B110" t="s">
+      <c r="B110" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C110" t="s">
         <v>109</v>
       </c>
-      <c r="C110" s="1" t="n"/>
-      <c r="D110" t="n">
-        <v>101</v>
-      </c>
+      <c r="D110" s="2" t="n"/>
     </row>
     <row r="111" spans="1:4">
-      <c r="B111" t="s">
+      <c r="B111" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C111" t="s">
         <v>110</v>
       </c>
-      <c r="C111" s="1" t="n"/>
-      <c r="D111" t="n">
-        <v>101</v>
-      </c>
+      <c r="D111" s="2" t="n"/>
     </row>
     <row r="112" spans="1:4">
-      <c r="B112" t="s">
+      <c r="B112" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C112" t="s">
         <v>111</v>
       </c>
-      <c r="C112" s="1" t="n"/>
-      <c r="D112" t="n">
-        <v>101</v>
-      </c>
+      <c r="D112" s="2" t="n"/>
     </row>
     <row r="113" spans="1:4">
-      <c r="B113" t="s">
+      <c r="B113" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C113" t="s">
         <v>112</v>
       </c>
-      <c r="C113" s="1" t="n"/>
-      <c r="D113" t="n">
-        <v>101</v>
-      </c>
+      <c r="D113" s="2" t="n"/>
     </row>
     <row r="114" spans="1:4">
-      <c r="B114" t="s">
+      <c r="B114" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C114" t="s">
         <v>113</v>
       </c>
-      <c r="C114" s="1" t="n"/>
-      <c r="D114" t="n">
-        <v>101</v>
-      </c>
+      <c r="D114" s="2" t="n"/>
     </row>
     <row r="115" spans="1:4">
-      <c r="B115" t="s">
+      <c r="B115" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C115" t="s">
         <v>114</v>
       </c>
-      <c r="C115" s="1" t="n"/>
-      <c r="D115" t="n">
-        <v>101</v>
-      </c>
+      <c r="D115" s="2" t="n"/>
     </row>
     <row r="116" spans="1:4">
-      <c r="B116" t="s">
+      <c r="B116" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C116" t="s">
         <v>115</v>
       </c>
-      <c r="C116" s="1" t="n"/>
-      <c r="D116" t="n">
-        <v>101</v>
-      </c>
+      <c r="D116" s="2" t="n"/>
     </row>
     <row r="117" spans="1:4">
-      <c r="B117" t="s">
+      <c r="B117" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C117" t="s">
         <v>116</v>
       </c>
-      <c r="C117" s="1" t="n"/>
-      <c r="D117" t="n">
-        <v>101</v>
-      </c>
+      <c r="D117" s="2" t="n"/>
     </row>
     <row r="118" spans="1:4">
-      <c r="B118" t="s">
+      <c r="B118" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C118" t="s">
         <v>117</v>
       </c>
-      <c r="C118" s="1" t="n"/>
-      <c r="D118" t="n">
-        <v>101</v>
-      </c>
+      <c r="D118" s="2" t="n"/>
     </row>
     <row r="119" spans="1:4">
-      <c r="B119" t="s">
+      <c r="B119" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C119" t="s">
         <v>118</v>
       </c>
-      <c r="C119" s="1" t="n"/>
-      <c r="D119" t="n">
-        <v>101</v>
-      </c>
+      <c r="D119" s="2" t="n"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="B120" t="s">
+      <c r="B120" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C120" t="s">
         <v>119</v>
       </c>
-      <c r="C120" s="1" t="n"/>
-      <c r="D120" t="n">
-        <v>101</v>
-      </c>
+      <c r="D120" s="2" t="n"/>
     </row>
     <row r="121" spans="1:4">
-      <c r="B121" t="s">
+      <c r="B121" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C121" t="s">
         <v>120</v>
       </c>
-      <c r="C121" s="1" t="n"/>
-      <c r="D121" t="n">
-        <v>101</v>
-      </c>
+      <c r="D121" s="2" t="n"/>
     </row>
     <row r="122" spans="1:4">
-      <c r="B122" t="s">
+      <c r="B122" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C122" t="s">
         <v>121</v>
       </c>
-      <c r="C122" s="1" t="n"/>
-      <c r="D122" t="n">
-        <v>101</v>
-      </c>
+      <c r="D122" s="2" t="n"/>
     </row>
     <row r="123" spans="1:4">
-      <c r="B123" t="s">
+      <c r="B123" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C123" t="s">
         <v>122</v>
       </c>
-      <c r="C123" s="1" t="n"/>
-      <c r="D123" t="n">
-        <v>101</v>
-      </c>
+      <c r="D123" s="2" t="n"/>
     </row>
     <row r="124" spans="1:4">
-      <c r="B124" t="s">
+      <c r="B124" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C124" t="s">
         <v>123</v>
       </c>
-      <c r="C124" s="1" t="n"/>
-      <c r="D124" t="n">
-        <v>101</v>
-      </c>
+      <c r="D124" s="2" t="n"/>
     </row>
     <row r="125" spans="1:4">
-      <c r="B125" t="s">
+      <c r="B125" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C125" t="s">
         <v>124</v>
       </c>
-      <c r="C125" s="1" t="n"/>
-      <c r="D125" t="n">
-        <v>101</v>
-      </c>
+      <c r="D125" s="2" t="n"/>
     </row>
     <row r="126" spans="1:4">
-      <c r="B126" t="s">
+      <c r="B126" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C126" t="s">
         <v>125</v>
       </c>
-      <c r="C126" s="1" t="n"/>
-      <c r="D126" t="n">
-        <v>101</v>
-      </c>
+      <c r="D126" s="2" t="n"/>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="B127" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C127" t="s">
+        <v>126</v>
+      </c>
+      <c r="D127" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Adds formatting - column width and bold, centered font
</commit_message>
<xml_diff>
--- a/OWGR.xlsx
+++ b/OWGR.xlsx
@@ -454,10 +454,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="justify"/>
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -778,7 +781,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="2" min="2" width="20"/>
+    <col customWidth="1" max="2" min="2" width="4"/>
+    <col customWidth="1" max="3" min="3" width="18"/>
+    <col customWidth="1" max="4" min="4" width="4"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -796,1117 +801,1117 @@
       <c r="B4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="n"/>
+      <c r="D4" s="3" t="n"/>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="n"/>
+      <c r="D5" s="3" t="n"/>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="n"/>
+      <c r="D6" s="3" t="n"/>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="2" t="n"/>
+      <c r="D7" s="3" t="n"/>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2" t="n"/>
+      <c r="D8" s="3" t="n"/>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2" t="n"/>
+      <c r="D9" s="3" t="n"/>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2" t="n"/>
+      <c r="D10" s="3" t="n"/>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="n"/>
+      <c r="D11" s="3" t="n"/>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="2" t="n"/>
+      <c r="D12" s="3" t="n"/>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="2" t="n"/>
+      <c r="D13" s="3" t="n"/>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="2" t="n"/>
+      <c r="D14" s="3" t="n"/>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="2" t="n"/>
+      <c r="D15" s="3" t="n"/>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="2" t="n"/>
+      <c r="D16" s="3" t="n"/>
     </row>
     <row r="17" spans="1:4">
       <c r="B17" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="2" t="n"/>
+      <c r="D17" s="3" t="n"/>
     </row>
     <row r="18" spans="1:4">
       <c r="B18" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="3" t="n"/>
+      <c r="D18" s="4" t="n"/>
     </row>
     <row r="19" spans="1:4">
       <c r="B19" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="2" t="n"/>
+      <c r="D19" s="3" t="n"/>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="2" t="n"/>
+      <c r="D20" s="3" t="n"/>
     </row>
     <row r="21" spans="1:4">
       <c r="B21" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="2" t="n"/>
+      <c r="D21" s="3" t="n"/>
     </row>
     <row r="22" spans="1:4">
       <c r="B22" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="2" t="n"/>
+      <c r="D22" s="3" t="n"/>
     </row>
     <row r="23" spans="1:4">
       <c r="B23" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="3" t="n"/>
+      <c r="D23" s="4" t="n"/>
     </row>
     <row r="24" spans="1:4">
       <c r="B24" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="3" t="n"/>
+      <c r="D24" s="4" t="n"/>
     </row>
     <row r="25" spans="1:4">
       <c r="B25" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="2" t="n"/>
+      <c r="D25" s="3" t="n"/>
     </row>
     <row r="26" spans="1:4">
       <c r="B26" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="3" t="n"/>
+      <c r="D26" s="4" t="n"/>
     </row>
     <row r="27" spans="1:4">
       <c r="B27" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="2" t="n"/>
+      <c r="D27" s="3" t="n"/>
     </row>
     <row r="28" spans="1:4">
       <c r="B28" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="3" t="n"/>
+      <c r="D28" s="4" t="n"/>
     </row>
     <row r="29" spans="1:4">
       <c r="B29" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="2" t="n"/>
+      <c r="D29" s="3" t="n"/>
     </row>
     <row r="30" spans="1:4">
       <c r="B30" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="2" t="n"/>
+      <c r="D30" s="3" t="n"/>
     </row>
     <row r="31" spans="1:4">
       <c r="B31" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="2" t="n"/>
+      <c r="D31" s="3" t="n"/>
     </row>
     <row r="32" spans="1:4">
       <c r="B32" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="2" t="n"/>
+      <c r="D32" s="3" t="n"/>
     </row>
     <row r="33" spans="1:4">
       <c r="B33" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="3" t="n"/>
+      <c r="D33" s="4" t="n"/>
     </row>
     <row r="34" spans="1:4">
       <c r="B34" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="2" t="n"/>
+      <c r="D34" s="3" t="n"/>
     </row>
     <row r="35" spans="1:4">
       <c r="B35" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="2" t="n"/>
+      <c r="D35" s="3" t="n"/>
     </row>
     <row r="36" spans="1:4">
       <c r="B36" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="3" t="n"/>
+      <c r="D36" s="4" t="n"/>
     </row>
     <row r="37" spans="1:4">
       <c r="B37" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="2" t="n"/>
+      <c r="D37" s="3" t="n"/>
     </row>
     <row r="38" spans="1:4">
       <c r="B38" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="2" t="n"/>
+      <c r="D38" s="3" t="n"/>
     </row>
     <row r="39" spans="1:4">
       <c r="B39" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="2" t="n"/>
+      <c r="D39" s="3" t="n"/>
     </row>
     <row r="40" spans="1:4">
       <c r="B40" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="3" t="n"/>
+      <c r="D40" s="4" t="n"/>
     </row>
     <row r="41" spans="1:4">
       <c r="B41" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="2" t="n"/>
+      <c r="D41" s="3" t="n"/>
     </row>
     <row r="42" spans="1:4">
       <c r="B42" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="3" t="n"/>
+      <c r="D42" s="4" t="n"/>
     </row>
     <row r="43" spans="1:4">
       <c r="B43" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="3" t="n"/>
+      <c r="D43" s="4" t="n"/>
     </row>
     <row r="44" spans="1:4">
       <c r="B44" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D44" s="3" t="n"/>
+      <c r="D44" s="4" t="n"/>
     </row>
     <row r="45" spans="1:4">
       <c r="B45" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="2" t="n"/>
+      <c r="D45" s="3" t="n"/>
     </row>
     <row r="46" spans="1:4">
       <c r="B46" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D46" s="3" t="n"/>
+      <c r="D46" s="4" t="n"/>
     </row>
     <row r="47" spans="1:4">
       <c r="B47" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D47" s="2" t="n"/>
+      <c r="D47" s="3" t="n"/>
     </row>
     <row r="48" spans="1:4">
       <c r="B48" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="2" t="n"/>
+      <c r="D48" s="3" t="n"/>
     </row>
     <row r="49" spans="1:4">
       <c r="B49" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D49" s="2" t="n"/>
+      <c r="D49" s="3" t="n"/>
     </row>
     <row r="50" spans="1:4">
       <c r="B50" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D50" s="2" t="n"/>
+      <c r="D50" s="3" t="n"/>
     </row>
     <row r="51" spans="1:4">
       <c r="B51" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D51" s="3" t="n"/>
+      <c r="D51" s="4" t="n"/>
     </row>
     <row r="52" spans="1:4">
       <c r="B52" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="3" t="n"/>
+      <c r="D52" s="4" t="n"/>
     </row>
     <row r="53" spans="1:4">
       <c r="B53" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D53" s="2" t="n"/>
+      <c r="D53" s="3" t="n"/>
     </row>
     <row r="54" spans="1:4">
       <c r="B54" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D54" s="3" t="n"/>
+      <c r="D54" s="4" t="n"/>
     </row>
     <row r="55" spans="1:4">
       <c r="B55" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D55" s="3" t="n"/>
+      <c r="D55" s="4" t="n"/>
     </row>
     <row r="56" spans="1:4">
       <c r="B56" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D56" s="3" t="n"/>
+      <c r="D56" s="4" t="n"/>
     </row>
     <row r="57" spans="1:4">
       <c r="B57" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D57" s="3" t="n"/>
+      <c r="D57" s="4" t="n"/>
     </row>
     <row r="58" spans="1:4">
       <c r="B58" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D58" s="2" t="n"/>
+      <c r="D58" s="3" t="n"/>
     </row>
     <row r="59" spans="1:4">
       <c r="B59" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D59" s="3" t="n"/>
+      <c r="D59" s="4" t="n"/>
     </row>
     <row r="60" spans="1:4">
       <c r="B60" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D60" s="2" t="n"/>
+      <c r="D60" s="3" t="n"/>
     </row>
     <row r="61" spans="1:4">
       <c r="B61" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D61" s="3" t="n"/>
+      <c r="D61" s="4" t="n"/>
     </row>
     <row r="62" spans="1:4">
       <c r="B62" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D62" s="3" t="n"/>
+      <c r="D62" s="4" t="n"/>
     </row>
     <row r="63" spans="1:4">
       <c r="B63" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D63" s="3" t="n"/>
+      <c r="D63" s="4" t="n"/>
     </row>
     <row r="64" spans="1:4">
       <c r="B64" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D64" s="3" t="n"/>
+      <c r="D64" s="4" t="n"/>
     </row>
     <row r="65" spans="1:4">
       <c r="B65" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D65" s="3" t="n"/>
+      <c r="D65" s="4" t="n"/>
     </row>
     <row r="66" spans="1:4">
       <c r="B66" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D66" s="2" t="n"/>
+      <c r="D66" s="3" t="n"/>
     </row>
     <row r="67" spans="1:4">
       <c r="B67" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D67" s="3" t="n"/>
+      <c r="D67" s="4" t="n"/>
     </row>
     <row r="68" spans="1:4">
       <c r="B68" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D68" s="3" t="n"/>
+      <c r="D68" s="4" t="n"/>
     </row>
     <row r="69" spans="1:4">
       <c r="B69" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D69" s="2" t="n"/>
+      <c r="D69" s="3" t="n"/>
     </row>
     <row r="70" spans="1:4">
       <c r="B70" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D70" s="2" t="n"/>
+      <c r="D70" s="3" t="n"/>
     </row>
     <row r="71" spans="1:4">
       <c r="B71" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D71" s="3" t="n"/>
+      <c r="D71" s="4" t="n"/>
     </row>
     <row r="72" spans="1:4">
       <c r="B72" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D72" s="2" t="n"/>
+      <c r="D72" s="3" t="n"/>
     </row>
     <row r="73" spans="1:4">
       <c r="B73" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D73" s="2" t="n"/>
+      <c r="D73" s="3" t="n"/>
     </row>
     <row r="74" spans="1:4">
       <c r="B74" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D74" s="3" t="n"/>
+      <c r="D74" s="4" t="n"/>
     </row>
     <row r="75" spans="1:4">
       <c r="B75" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D75" s="2" t="n"/>
+      <c r="D75" s="3" t="n"/>
     </row>
     <row r="76" spans="1:4">
       <c r="B76" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D76" s="3" t="n"/>
+      <c r="D76" s="4" t="n"/>
     </row>
     <row r="77" spans="1:4">
       <c r="B77" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D77" s="2" t="n"/>
+      <c r="D77" s="3" t="n"/>
     </row>
     <row r="78" spans="1:4">
       <c r="B78" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D78" s="2" t="n"/>
+      <c r="D78" s="3" t="n"/>
     </row>
     <row r="79" spans="1:4">
       <c r="B79" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D79" s="3" t="n"/>
+      <c r="D79" s="4" t="n"/>
     </row>
     <row r="80" spans="1:4">
       <c r="B80" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D80" s="3" t="n"/>
+      <c r="D80" s="4" t="n"/>
     </row>
     <row r="81" spans="1:4">
       <c r="B81" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D81" s="2" t="n"/>
+      <c r="D81" s="3" t="n"/>
     </row>
     <row r="82" spans="1:4">
       <c r="B82" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D82" s="3" t="n"/>
+      <c r="D82" s="4" t="n"/>
     </row>
     <row r="83" spans="1:4">
       <c r="B83" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D83" s="3" t="n"/>
+      <c r="D83" s="4" t="n"/>
     </row>
     <row r="84" spans="1:4">
       <c r="B84" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D84" s="2" t="n"/>
+      <c r="D84" s="3" t="n"/>
     </row>
     <row r="85" spans="1:4">
       <c r="B85" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D85" s="2" t="n"/>
+      <c r="D85" s="3" t="n"/>
     </row>
     <row r="86" spans="1:4">
       <c r="B86" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D86" s="3" t="n"/>
+      <c r="D86" s="4" t="n"/>
     </row>
     <row r="87" spans="1:4">
       <c r="B87" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D87" s="2" t="n"/>
+      <c r="D87" s="3" t="n"/>
     </row>
     <row r="88" spans="1:4">
       <c r="B88" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D88" s="2" t="n"/>
+      <c r="D88" s="3" t="n"/>
     </row>
     <row r="89" spans="1:4">
       <c r="B89" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D89" s="3" t="n"/>
+      <c r="D89" s="4" t="n"/>
     </row>
     <row r="90" spans="1:4">
       <c r="B90" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D90" s="3" t="n"/>
+      <c r="D90" s="4" t="n"/>
     </row>
     <row r="91" spans="1:4">
       <c r="B91" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D91" s="3" t="n"/>
+      <c r="D91" s="4" t="n"/>
     </row>
     <row r="92" spans="1:4">
       <c r="B92" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D92" s="3" t="n"/>
+      <c r="D92" s="4" t="n"/>
     </row>
     <row r="93" spans="1:4">
       <c r="B93" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D93" s="2" t="n"/>
+      <c r="D93" s="3" t="n"/>
     </row>
     <row r="94" spans="1:4">
       <c r="B94" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D94" s="3" t="n"/>
+      <c r="D94" s="4" t="n"/>
     </row>
     <row r="95" spans="1:4">
       <c r="B95" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D95" s="3" t="n"/>
+      <c r="D95" s="4" t="n"/>
     </row>
     <row r="96" spans="1:4">
       <c r="B96" s="1" t="n">
         <v>93</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D96" s="2" t="n"/>
+      <c r="D96" s="3" t="n"/>
     </row>
     <row r="97" spans="1:4">
       <c r="B97" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D97" s="3" t="n"/>
+      <c r="D97" s="4" t="n"/>
     </row>
     <row r="98" spans="1:4">
       <c r="B98" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D98" s="2" t="n"/>
+      <c r="D98" s="3" t="n"/>
     </row>
     <row r="99" spans="1:4">
       <c r="B99" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D99" s="3" t="n"/>
+      <c r="D99" s="4" t="n"/>
     </row>
     <row r="100" spans="1:4">
       <c r="B100" s="1" t="n">
         <v>97</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D100" s="3" t="n"/>
+      <c r="D100" s="4" t="n"/>
     </row>
     <row r="101" spans="1:4">
       <c r="B101" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D101" s="3" t="n"/>
+      <c r="D101" s="4" t="n"/>
     </row>
     <row r="102" spans="1:4">
       <c r="B102" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="C102" t="s">
-        <v>101</v>
-      </c>
-      <c r="D102" s="3" t="n"/>
+      <c r="C102" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D102" s="4" t="n"/>
     </row>
     <row r="103" spans="1:4">
       <c r="B103" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D103" s="3" t="n"/>
+      <c r="D103" s="4" t="n"/>
     </row>
     <row r="104" spans="1:4">
       <c r="B104" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D104" s="3" t="n"/>
+      <c r="D104" s="4" t="n"/>
     </row>
     <row r="105" spans="1:4">
       <c r="B105" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D105" s="3" t="n"/>
+      <c r="D105" s="4" t="n"/>
     </row>
     <row r="106" spans="1:4">
       <c r="B106" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D106" s="2" t="n"/>
+      <c r="D106" s="3" t="n"/>
     </row>
     <row r="107" spans="1:4">
       <c r="B107" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D107" s="2" t="n"/>
+      <c r="D107" s="3" t="n"/>
     </row>
     <row r="108" spans="1:4">
       <c r="B108" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D108" s="2" t="n"/>
+      <c r="D108" s="3" t="n"/>
     </row>
     <row r="109" spans="1:4">
       <c r="B109" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D109" s="2" t="n"/>
+      <c r="D109" s="3" t="n"/>
     </row>
     <row r="110" spans="1:4">
       <c r="B110" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D110" s="2" t="n"/>
+      <c r="D110" s="3" t="n"/>
     </row>
     <row r="111" spans="1:4">
       <c r="B111" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D111" s="2" t="n"/>
+      <c r="D111" s="3" t="n"/>
     </row>
     <row r="112" spans="1:4">
       <c r="B112" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D112" s="2" t="n"/>
+      <c r="D112" s="3" t="n"/>
     </row>
     <row r="113" spans="1:4">
       <c r="B113" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D113" s="2" t="n"/>
+      <c r="D113" s="3" t="n"/>
     </row>
     <row r="114" spans="1:4">
       <c r="B114" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D114" s="2" t="n"/>
+      <c r="D114" s="3" t="n"/>
     </row>
     <row r="115" spans="1:4">
       <c r="B115" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D115" s="2" t="n"/>
+      <c r="D115" s="3" t="n"/>
     </row>
     <row r="116" spans="1:4">
       <c r="B116" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D116" s="2" t="n"/>
+      <c r="D116" s="3" t="n"/>
     </row>
     <row r="117" spans="1:4">
       <c r="B117" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D117" s="2" t="n"/>
+      <c r="D117" s="3" t="n"/>
     </row>
     <row r="118" spans="1:4">
       <c r="B118" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D118" s="2" t="n"/>
+      <c r="D118" s="3" t="n"/>
     </row>
     <row r="119" spans="1:4">
       <c r="B119" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D119" s="2" t="n"/>
+      <c r="D119" s="3" t="n"/>
     </row>
     <row r="120" spans="1:4">
       <c r="B120" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D120" s="2" t="n"/>
+      <c r="D120" s="3" t="n"/>
     </row>
     <row r="121" spans="1:4">
       <c r="B121" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D121" s="2" t="n"/>
+      <c r="D121" s="3" t="n"/>
     </row>
     <row r="122" spans="1:4">
       <c r="B122" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D122" s="2" t="n"/>
+      <c r="D122" s="3" t="n"/>
     </row>
     <row r="123" spans="1:4">
       <c r="B123" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D123" s="2" t="n"/>
+      <c r="D123" s="3" t="n"/>
     </row>
     <row r="124" spans="1:4">
       <c r="B124" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C124" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D124" s="2" t="n"/>
+      <c r="D124" s="3" t="n"/>
     </row>
     <row r="125" spans="1:4">
       <c r="B125" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D125" s="2" t="n"/>
+      <c r="D125" s="3" t="n"/>
     </row>
     <row r="126" spans="1:4">
       <c r="B126" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C126" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D126" s="2" t="n"/>
+      <c r="D126" s="3" t="n"/>
     </row>
     <row r="127" spans="1:4">
       <c r="B127" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D127" s="2" t="n"/>
+      <c r="D127" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Refined formatting. Adds thick line at rank 64.
</commit_message>
<xml_diff>
--- a/OWGR.xlsx
+++ b/OWGR.xlsx
@@ -413,6 +413,7 @@
     </font>
     <font>
       <b val="1"/>
+      <sz val="14"/>
     </font>
   </fonts>
   <fills count="4">
@@ -435,7 +436,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -444,17 +445,24 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thick"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" shrinkToFit="1"/>
@@ -464,6 +472,14 @@
     </xf>
     <xf borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -773,7 +789,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:D127"/>
+  <dimension ref="A3:E127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -781,12 +797,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="2" min="2" width="4"/>
-    <col customWidth="1" max="3" min="3" width="18"/>
-    <col customWidth="1" max="4" min="4" width="4"/>
+    <col customWidth="1" max="2" min="2" width="6"/>
+    <col customWidth="1" max="3" min="3" width="20"/>
+    <col customWidth="1" max="4" min="4" width="6"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -797,7 +813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="B4" s="1" t="n">
         <v>1</v>
       </c>
@@ -806,7 +822,7 @@
       </c>
       <c r="D4" s="3" t="n"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="B5" s="1" t="n">
         <v>2</v>
       </c>
@@ -815,7 +831,7 @@
       </c>
       <c r="D5" s="3" t="n"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="B6" s="1" t="n">
         <v>3</v>
       </c>
@@ -824,7 +840,7 @@
       </c>
       <c r="D6" s="3" t="n"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="B7" s="1" t="n">
         <v>4</v>
       </c>
@@ -833,7 +849,7 @@
       </c>
       <c r="D7" s="3" t="n"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="B8" s="1" t="n">
         <v>5</v>
       </c>
@@ -842,7 +858,7 @@
       </c>
       <c r="D8" s="3" t="n"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="B9" s="1" t="n">
         <v>6</v>
       </c>
@@ -851,7 +867,7 @@
       </c>
       <c r="D9" s="3" t="n"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="B10" s="1" t="n">
         <v>7</v>
       </c>
@@ -860,7 +876,7 @@
       </c>
       <c r="D10" s="3" t="n"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="B11" s="1" t="n">
         <v>8</v>
       </c>
@@ -869,7 +885,7 @@
       </c>
       <c r="D11" s="3" t="n"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="B12" s="1" t="n">
         <v>9</v>
       </c>
@@ -878,7 +894,7 @@
       </c>
       <c r="D12" s="3" t="n"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="B13" s="1" t="n">
         <v>10</v>
       </c>
@@ -887,7 +903,7 @@
       </c>
       <c r="D13" s="3" t="n"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="B14" s="1" t="n">
         <v>11</v>
       </c>
@@ -896,7 +912,7 @@
       </c>
       <c r="D14" s="3" t="n"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="B15" s="1" t="n">
         <v>12</v>
       </c>
@@ -905,7 +921,7 @@
       </c>
       <c r="D15" s="3" t="n"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="B16" s="1" t="n">
         <v>13</v>
       </c>
@@ -914,7 +930,7 @@
       </c>
       <c r="D16" s="3" t="n"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="B17" s="1" t="n">
         <v>14</v>
       </c>
@@ -923,7 +939,7 @@
       </c>
       <c r="D17" s="3" t="n"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="B18" s="1" t="n">
         <v>15</v>
       </c>
@@ -932,7 +948,7 @@
       </c>
       <c r="D18" s="4" t="n"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="B19" s="1" t="n">
         <v>16</v>
       </c>
@@ -941,7 +957,7 @@
       </c>
       <c r="D19" s="3" t="n"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="B20" s="1" t="n">
         <v>17</v>
       </c>
@@ -950,7 +966,7 @@
       </c>
       <c r="D20" s="3" t="n"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="B21" s="1" t="n">
         <v>18</v>
       </c>
@@ -959,7 +975,7 @@
       </c>
       <c r="D21" s="3" t="n"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="B22" s="1" t="n">
         <v>19</v>
       </c>
@@ -968,7 +984,7 @@
       </c>
       <c r="D22" s="3" t="n"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="B23" s="1" t="n">
         <v>20</v>
       </c>
@@ -977,7 +993,7 @@
       </c>
       <c r="D23" s="4" t="n"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="B24" s="1" t="n">
         <v>21</v>
       </c>
@@ -986,7 +1002,7 @@
       </c>
       <c r="D24" s="4" t="n"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="B25" s="1" t="n">
         <v>22</v>
       </c>
@@ -995,7 +1011,7 @@
       </c>
       <c r="D25" s="3" t="n"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="B26" s="1" t="n">
         <v>23</v>
       </c>
@@ -1004,7 +1020,7 @@
       </c>
       <c r="D26" s="4" t="n"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="B27" s="1" t="n">
         <v>24</v>
       </c>
@@ -1013,7 +1029,7 @@
       </c>
       <c r="D27" s="3" t="n"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="B28" s="1" t="n">
         <v>25</v>
       </c>
@@ -1022,7 +1038,7 @@
       </c>
       <c r="D28" s="4" t="n"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="B29" s="1" t="n">
         <v>26</v>
       </c>
@@ -1031,7 +1047,7 @@
       </c>
       <c r="D29" s="3" t="n"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="B30" s="1" t="n">
         <v>27</v>
       </c>
@@ -1040,7 +1056,7 @@
       </c>
       <c r="D30" s="3" t="n"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="B31" s="1" t="n">
         <v>28</v>
       </c>
@@ -1049,7 +1065,7 @@
       </c>
       <c r="D31" s="3" t="n"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="B32" s="1" t="n">
         <v>29</v>
       </c>
@@ -1058,7 +1074,7 @@
       </c>
       <c r="D32" s="3" t="n"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="B33" s="1" t="n">
         <v>30</v>
       </c>
@@ -1067,7 +1083,7 @@
       </c>
       <c r="D33" s="4" t="n"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="B34" s="1" t="n">
         <v>31</v>
       </c>
@@ -1076,7 +1092,7 @@
       </c>
       <c r="D34" s="3" t="n"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5">
       <c r="B35" s="1" t="n">
         <v>32</v>
       </c>
@@ -1085,7 +1101,7 @@
       </c>
       <c r="D35" s="3" t="n"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="B36" s="1" t="n">
         <v>33</v>
       </c>
@@ -1094,7 +1110,7 @@
       </c>
       <c r="D36" s="4" t="n"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="B37" s="1" t="n">
         <v>34</v>
       </c>
@@ -1103,7 +1119,7 @@
       </c>
       <c r="D37" s="3" t="n"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="B38" s="1" t="n">
         <v>35</v>
       </c>
@@ -1112,7 +1128,7 @@
       </c>
       <c r="D38" s="3" t="n"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="B39" s="1" t="n">
         <v>36</v>
       </c>
@@ -1121,7 +1137,7 @@
       </c>
       <c r="D39" s="3" t="n"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="B40" s="1" t="n">
         <v>37</v>
       </c>
@@ -1130,7 +1146,7 @@
       </c>
       <c r="D40" s="4" t="n"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5">
       <c r="B41" s="1" t="n">
         <v>38</v>
       </c>
@@ -1139,7 +1155,7 @@
       </c>
       <c r="D41" s="3" t="n"/>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5">
       <c r="B42" s="1" t="n">
         <v>39</v>
       </c>
@@ -1148,7 +1164,7 @@
       </c>
       <c r="D42" s="4" t="n"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:5">
       <c r="B43" s="1" t="n">
         <v>40</v>
       </c>
@@ -1157,7 +1173,7 @@
       </c>
       <c r="D43" s="4" t="n"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="B44" s="1" t="n">
         <v>41</v>
       </c>
@@ -1166,7 +1182,7 @@
       </c>
       <c r="D44" s="4" t="n"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:5">
       <c r="B45" s="1" t="n">
         <v>42</v>
       </c>
@@ -1175,7 +1191,7 @@
       </c>
       <c r="D45" s="3" t="n"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="B46" s="1" t="n">
         <v>43</v>
       </c>
@@ -1184,7 +1200,7 @@
       </c>
       <c r="D46" s="4" t="n"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:5">
       <c r="B47" s="1" t="n">
         <v>44</v>
       </c>
@@ -1193,7 +1209,7 @@
       </c>
       <c r="D47" s="3" t="n"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:5">
       <c r="B48" s="1" t="n">
         <v>45</v>
       </c>
@@ -1202,7 +1218,7 @@
       </c>
       <c r="D48" s="3" t="n"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:5">
       <c r="B49" s="1" t="n">
         <v>46</v>
       </c>
@@ -1211,7 +1227,7 @@
       </c>
       <c r="D49" s="3" t="n"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:5">
       <c r="B50" s="1" t="n">
         <v>47</v>
       </c>
@@ -1220,7 +1236,7 @@
       </c>
       <c r="D50" s="3" t="n"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:5">
       <c r="B51" s="1" t="n">
         <v>48</v>
       </c>
@@ -1229,7 +1245,7 @@
       </c>
       <c r="D51" s="4" t="n"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:5">
       <c r="B52" s="1" t="n">
         <v>49</v>
       </c>
@@ -1238,7 +1254,7 @@
       </c>
       <c r="D52" s="4" t="n"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:5">
       <c r="B53" s="1" t="n">
         <v>50</v>
       </c>
@@ -1247,7 +1263,7 @@
       </c>
       <c r="D53" s="3" t="n"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:5">
       <c r="B54" s="1" t="n">
         <v>51</v>
       </c>
@@ -1256,7 +1272,7 @@
       </c>
       <c r="D54" s="4" t="n"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:5">
       <c r="B55" s="1" t="n">
         <v>52</v>
       </c>
@@ -1265,7 +1281,7 @@
       </c>
       <c r="D55" s="4" t="n"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:5">
       <c r="B56" s="1" t="n">
         <v>53</v>
       </c>
@@ -1274,7 +1290,7 @@
       </c>
       <c r="D56" s="4" t="n"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:5">
       <c r="B57" s="1" t="n">
         <v>54</v>
       </c>
@@ -1283,7 +1299,7 @@
       </c>
       <c r="D57" s="4" t="n"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:5">
       <c r="B58" s="1" t="n">
         <v>55</v>
       </c>
@@ -1292,7 +1308,7 @@
       </c>
       <c r="D58" s="3" t="n"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:5">
       <c r="B59" s="1" t="n">
         <v>56</v>
       </c>
@@ -1301,7 +1317,7 @@
       </c>
       <c r="D59" s="4" t="n"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:5">
       <c r="B60" s="1" t="n">
         <v>57</v>
       </c>
@@ -1310,7 +1326,7 @@
       </c>
       <c r="D60" s="3" t="n"/>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:5">
       <c r="B61" s="1" t="n">
         <v>58</v>
       </c>
@@ -1319,7 +1335,7 @@
       </c>
       <c r="D61" s="4" t="n"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:5">
       <c r="B62" s="1" t="n">
         <v>59</v>
       </c>
@@ -1328,7 +1344,7 @@
       </c>
       <c r="D62" s="4" t="n"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:5">
       <c r="B63" s="1" t="n">
         <v>60</v>
       </c>
@@ -1337,7 +1353,7 @@
       </c>
       <c r="D63" s="4" t="n"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:5">
       <c r="B64" s="1" t="n">
         <v>61</v>
       </c>
@@ -1346,7 +1362,7 @@
       </c>
       <c r="D64" s="4" t="n"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:5">
       <c r="B65" s="1" t="n">
         <v>62</v>
       </c>
@@ -1355,7 +1371,7 @@
       </c>
       <c r="D65" s="4" t="n"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:5">
       <c r="B66" s="1" t="n">
         <v>63</v>
       </c>
@@ -1364,16 +1380,18 @@
       </c>
       <c r="D66" s="3" t="n"/>
     </row>
-    <row r="67" spans="1:4">
-      <c r="B67" s="1" t="n">
+    <row r="67" spans="1:5">
+      <c r="A67" s="5" t="n"/>
+      <c r="B67" s="6" t="n">
         <v>64</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D67" s="4" t="n"/>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="D67" s="8" t="n"/>
+      <c r="E67" s="5" t="n"/>
+    </row>
+    <row r="68" spans="1:5">
       <c r="B68" s="1" t="n">
         <v>65</v>
       </c>
@@ -1382,7 +1400,7 @@
       </c>
       <c r="D68" s="4" t="n"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:5">
       <c r="B69" s="1" t="n">
         <v>66</v>
       </c>
@@ -1391,7 +1409,7 @@
       </c>
       <c r="D69" s="3" t="n"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:5">
       <c r="B70" s="1" t="n">
         <v>67</v>
       </c>
@@ -1400,7 +1418,7 @@
       </c>
       <c r="D70" s="3" t="n"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:5">
       <c r="B71" s="1" t="n">
         <v>68</v>
       </c>
@@ -1409,7 +1427,7 @@
       </c>
       <c r="D71" s="4" t="n"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:5">
       <c r="B72" s="1" t="n">
         <v>69</v>
       </c>
@@ -1418,7 +1436,7 @@
       </c>
       <c r="D72" s="3" t="n"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:5">
       <c r="B73" s="1" t="n">
         <v>70</v>
       </c>
@@ -1427,7 +1445,7 @@
       </c>
       <c r="D73" s="3" t="n"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:5">
       <c r="B74" s="1" t="n">
         <v>71</v>
       </c>
@@ -1436,7 +1454,7 @@
       </c>
       <c r="D74" s="4" t="n"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:5">
       <c r="B75" s="1" t="n">
         <v>72</v>
       </c>
@@ -1445,7 +1463,7 @@
       </c>
       <c r="D75" s="3" t="n"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:5">
       <c r="B76" s="1" t="n">
         <v>73</v>
       </c>
@@ -1454,7 +1472,7 @@
       </c>
       <c r="D76" s="4" t="n"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:5">
       <c r="B77" s="1" t="n">
         <v>74</v>
       </c>
@@ -1463,7 +1481,7 @@
       </c>
       <c r="D77" s="3" t="n"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:5">
       <c r="B78" s="1" t="n">
         <v>75</v>
       </c>
@@ -1472,7 +1490,7 @@
       </c>
       <c r="D78" s="3" t="n"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:5">
       <c r="B79" s="1" t="n">
         <v>76</v>
       </c>
@@ -1481,7 +1499,7 @@
       </c>
       <c r="D79" s="4" t="n"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:5">
       <c r="B80" s="1" t="n">
         <v>77</v>
       </c>
@@ -1490,7 +1508,7 @@
       </c>
       <c r="D80" s="4" t="n"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:5">
       <c r="B81" s="1" t="n">
         <v>78</v>
       </c>
@@ -1499,7 +1517,7 @@
       </c>
       <c r="D81" s="3" t="n"/>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:5">
       <c r="B82" s="1" t="n">
         <v>79</v>
       </c>
@@ -1508,7 +1526,7 @@
       </c>
       <c r="D82" s="4" t="n"/>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:5">
       <c r="B83" s="1" t="n">
         <v>80</v>
       </c>
@@ -1517,7 +1535,7 @@
       </c>
       <c r="D83" s="4" t="n"/>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:5">
       <c r="B84" s="1" t="n">
         <v>81</v>
       </c>
@@ -1526,7 +1544,7 @@
       </c>
       <c r="D84" s="3" t="n"/>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:5">
       <c r="B85" s="1" t="n">
         <v>82</v>
       </c>
@@ -1535,7 +1553,7 @@
       </c>
       <c r="D85" s="3" t="n"/>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:5">
       <c r="B86" s="1" t="n">
         <v>83</v>
       </c>
@@ -1544,7 +1562,7 @@
       </c>
       <c r="D86" s="4" t="n"/>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:5">
       <c r="B87" s="1" t="n">
         <v>84</v>
       </c>
@@ -1553,7 +1571,7 @@
       </c>
       <c r="D87" s="3" t="n"/>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:5">
       <c r="B88" s="1" t="n">
         <v>85</v>
       </c>
@@ -1562,7 +1580,7 @@
       </c>
       <c r="D88" s="3" t="n"/>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:5">
       <c r="B89" s="1" t="n">
         <v>86</v>
       </c>
@@ -1571,7 +1589,7 @@
       </c>
       <c r="D89" s="4" t="n"/>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:5">
       <c r="B90" s="1" t="n">
         <v>87</v>
       </c>
@@ -1580,7 +1598,7 @@
       </c>
       <c r="D90" s="4" t="n"/>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:5">
       <c r="B91" s="1" t="n">
         <v>88</v>
       </c>
@@ -1589,7 +1607,7 @@
       </c>
       <c r="D91" s="4" t="n"/>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:5">
       <c r="B92" s="1" t="n">
         <v>89</v>
       </c>
@@ -1598,7 +1616,7 @@
       </c>
       <c r="D92" s="4" t="n"/>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:5">
       <c r="B93" s="1" t="n">
         <v>90</v>
       </c>
@@ -1607,7 +1625,7 @@
       </c>
       <c r="D93" s="3" t="n"/>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:5">
       <c r="B94" s="1" t="n">
         <v>91</v>
       </c>
@@ -1616,7 +1634,7 @@
       </c>
       <c r="D94" s="4" t="n"/>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:5">
       <c r="B95" s="1" t="n">
         <v>92</v>
       </c>
@@ -1625,7 +1643,7 @@
       </c>
       <c r="D95" s="4" t="n"/>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:5">
       <c r="B96" s="1" t="n">
         <v>93</v>
       </c>
@@ -1634,7 +1652,7 @@
       </c>
       <c r="D96" s="3" t="n"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:5">
       <c r="B97" s="1" t="n">
         <v>94</v>
       </c>
@@ -1643,7 +1661,7 @@
       </c>
       <c r="D97" s="4" t="n"/>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:5">
       <c r="B98" s="1" t="n">
         <v>95</v>
       </c>
@@ -1652,7 +1670,7 @@
       </c>
       <c r="D98" s="3" t="n"/>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:5">
       <c r="B99" s="1" t="n">
         <v>96</v>
       </c>
@@ -1661,7 +1679,7 @@
       </c>
       <c r="D99" s="4" t="n"/>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:5">
       <c r="B100" s="1" t="n">
         <v>97</v>
       </c>
@@ -1670,7 +1688,7 @@
       </c>
       <c r="D100" s="4" t="n"/>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:5">
       <c r="B101" s="1" t="n">
         <v>98</v>
       </c>
@@ -1679,7 +1697,7 @@
       </c>
       <c r="D101" s="4" t="n"/>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:5">
       <c r="B102" s="1" t="n">
         <v>99</v>
       </c>
@@ -1688,7 +1706,7 @@
       </c>
       <c r="D102" s="4" t="n"/>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:5">
       <c r="B103" s="1" t="n">
         <v>100</v>
       </c>
@@ -1697,7 +1715,7 @@
       </c>
       <c r="D103" s="4" t="n"/>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:5">
       <c r="B104" s="1" t="n">
         <v>101</v>
       </c>
@@ -1706,7 +1724,7 @@
       </c>
       <c r="D104" s="4" t="n"/>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:5">
       <c r="B105" s="1" t="n">
         <v>101</v>
       </c>
@@ -1715,7 +1733,7 @@
       </c>
       <c r="D105" s="4" t="n"/>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:5">
       <c r="B106" s="1" t="n">
         <v>101</v>
       </c>
@@ -1724,7 +1742,7 @@
       </c>
       <c r="D106" s="3" t="n"/>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:5">
       <c r="B107" s="1" t="n">
         <v>101</v>
       </c>
@@ -1733,7 +1751,7 @@
       </c>
       <c r="D107" s="3" t="n"/>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:5">
       <c r="B108" s="1" t="n">
         <v>101</v>
       </c>
@@ -1742,7 +1760,7 @@
       </c>
       <c r="D108" s="3" t="n"/>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:5">
       <c r="B109" s="1" t="n">
         <v>101</v>
       </c>
@@ -1751,7 +1769,7 @@
       </c>
       <c r="D109" s="3" t="n"/>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:5">
       <c r="B110" s="1" t="n">
         <v>101</v>
       </c>
@@ -1760,7 +1778,7 @@
       </c>
       <c r="D110" s="3" t="n"/>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:5">
       <c r="B111" s="1" t="n">
         <v>101</v>
       </c>
@@ -1769,7 +1787,7 @@
       </c>
       <c r="D111" s="3" t="n"/>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:5">
       <c r="B112" s="1" t="n">
         <v>101</v>
       </c>
@@ -1778,7 +1796,7 @@
       </c>
       <c r="D112" s="3" t="n"/>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:5">
       <c r="B113" s="1" t="n">
         <v>101</v>
       </c>
@@ -1787,7 +1805,7 @@
       </c>
       <c r="D113" s="3" t="n"/>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:5">
       <c r="B114" s="1" t="n">
         <v>101</v>
       </c>
@@ -1796,7 +1814,7 @@
       </c>
       <c r="D114" s="3" t="n"/>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:5">
       <c r="B115" s="1" t="n">
         <v>101</v>
       </c>
@@ -1805,7 +1823,7 @@
       </c>
       <c r="D115" s="3" t="n"/>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:5">
       <c r="B116" s="1" t="n">
         <v>101</v>
       </c>
@@ -1814,7 +1832,7 @@
       </c>
       <c r="D116" s="3" t="n"/>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:5">
       <c r="B117" s="1" t="n">
         <v>101</v>
       </c>
@@ -1823,7 +1841,7 @@
       </c>
       <c r="D117" s="3" t="n"/>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:5">
       <c r="B118" s="1" t="n">
         <v>101</v>
       </c>
@@ -1832,7 +1850,7 @@
       </c>
       <c r="D118" s="3" t="n"/>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:5">
       <c r="B119" s="1" t="n">
         <v>101</v>
       </c>
@@ -1841,7 +1859,7 @@
       </c>
       <c r="D119" s="3" t="n"/>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:5">
       <c r="B120" s="1" t="n">
         <v>101</v>
       </c>
@@ -1850,7 +1868,7 @@
       </c>
       <c r="D120" s="3" t="n"/>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:5">
       <c r="B121" s="1" t="n">
         <v>101</v>
       </c>
@@ -1859,7 +1877,7 @@
       </c>
       <c r="D121" s="3" t="n"/>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:5">
       <c r="B122" s="1" t="n">
         <v>101</v>
       </c>
@@ -1868,7 +1886,7 @@
       </c>
       <c r="D122" s="3" t="n"/>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:5">
       <c r="B123" s="1" t="n">
         <v>101</v>
       </c>
@@ -1877,7 +1895,7 @@
       </c>
       <c r="D123" s="3" t="n"/>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:5">
       <c r="B124" s="1" t="n">
         <v>101</v>
       </c>
@@ -1886,7 +1904,7 @@
       </c>
       <c r="D124" s="3" t="n"/>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:5">
       <c r="B125" s="1" t="n">
         <v>101</v>
       </c>
@@ -1895,7 +1913,7 @@
       </c>
       <c r="D125" s="3" t="n"/>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:5">
       <c r="B126" s="1" t="n">
         <v>101</v>
       </c>
@@ -1904,7 +1922,7 @@
       </c>
       <c r="D126" s="3" t="n"/>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:5">
       <c r="B127" s="1" t="n">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
saves the list of all players into repository
</commit_message>
<xml_diff>
--- a/OWGR.xlsx
+++ b/OWGR.xlsx
@@ -59,12 +59,12 @@
     <t>Garcia, Sergio</t>
   </si>
   <si>
+    <t>Fleetwood, Tommy</t>
+  </si>
+  <si>
     <t>Stenson, Henrik</t>
   </si>
   <si>
-    <t>Fleetwood, Tommy</t>
-  </si>
-  <si>
     <t>Leishman, Marc</t>
   </si>
   <si>
@@ -74,33 +74,33 @@
     <t>Noren, Alex</t>
   </si>
   <si>
+    <t>Kuchar, Matt</t>
+  </si>
+  <si>
+    <t>Perez, Pat</t>
+  </si>
+  <si>
     <t>Casey, Paul</t>
   </si>
   <si>
-    <t>Kuchar, Matt</t>
-  </si>
-  <si>
-    <t>Perez, Pat</t>
-  </si>
-  <si>
     <t>Cabrera Bello, Rafael</t>
   </si>
   <si>
     <t>Harman, Brian</t>
   </si>
   <si>
+    <t>Schauffele, Xander</t>
+  </si>
+  <si>
+    <t>Hoffman, Charley</t>
+  </si>
+  <si>
     <t>Molinari, Francesco</t>
   </si>
   <si>
-    <t>Hoffman, Charley</t>
-  </si>
-  <si>
     <t>Reed, Patrick</t>
   </si>
   <si>
-    <t>Schauffele, Xander</t>
-  </si>
-  <si>
     <t>Woodland, Gary</t>
   </si>
   <si>
@@ -119,40 +119,52 @@
     <t>Kisner, Kevin</t>
   </si>
   <si>
+    <t>Mickelson, Phil</t>
+  </si>
+  <si>
+    <t>Finau, Tony</t>
+  </si>
+  <si>
+    <t>Cantlay, Patrick</t>
+  </si>
+  <si>
     <t>Berger, Daniel</t>
   </si>
   <si>
+    <t>Chappell, Kevin</t>
+  </si>
+  <si>
     <t>Haotong, Li</t>
   </si>
   <si>
-    <t>Chappell, Kevin</t>
-  </si>
-  <si>
-    <t>Mickelson, Phil</t>
+    <t>Aphibarnrat, Kiradech</t>
   </si>
   <si>
     <t>Steele, Brendan</t>
   </si>
   <si>
-    <t>Aphibarnrat, Kiradech</t>
+    <t>Watson, Bubba</t>
+  </si>
+  <si>
+    <t>Kodaira, Satoshi</t>
   </si>
   <si>
     <t>Pieters, Thomas</t>
   </si>
   <si>
-    <t>Cantlay, Patrick</t>
-  </si>
-  <si>
-    <t>Kodaira, Satoshi</t>
-  </si>
-  <si>
-    <t>Finau, Tony</t>
+    <t>Reavie, Chez</t>
+  </si>
+  <si>
+    <t>Dufner, Jason</t>
   </si>
   <si>
     <t>Simpson, Webb</t>
   </si>
   <si>
-    <t>Reavie, Chez</t>
+    <t>Ikeda, Yuta</t>
+  </si>
+  <si>
+    <t>Frittelli, Dylan</t>
   </si>
   <si>
     <t>Schwartzel, Charl</t>
@@ -161,69 +173,69 @@
     <t>Vegas, Jhonattan</t>
   </si>
   <si>
-    <t>Ikeda, Yuta</t>
-  </si>
-  <si>
-    <t>Dufner, Jason</t>
+    <t>Hadwin, Adam</t>
   </si>
   <si>
     <t>Kim, Siwoo</t>
   </si>
   <si>
-    <t>Frittelli, Dylan</t>
+    <t>Smith, Cameron</t>
   </si>
   <si>
     <t>Wiesberger, Bernd</t>
   </si>
   <si>
+    <t>Miyazato, Yusaku</t>
+  </si>
+  <si>
+    <t>Henley, Russell</t>
+  </si>
+  <si>
+    <t>Stanley, Kyle</t>
+  </si>
+  <si>
+    <t>Hahn, James</t>
+  </si>
+  <si>
     <t>Scott, Adam</t>
   </si>
   <si>
-    <t>Miyazato, Yusaku</t>
-  </si>
-  <si>
-    <t>Stanley, Kyle</t>
-  </si>
-  <si>
-    <t>Henley, Russell</t>
-  </si>
-  <si>
     <t>Johnson, Zach</t>
   </si>
   <si>
     <t>Kizzire, Patton</t>
   </si>
   <si>
-    <t>Hadwin, Adam</t>
-  </si>
-  <si>
-    <t>Smith, Cameron</t>
+    <t>Poulter, Ian</t>
   </si>
   <si>
     <t>Uihlein, Peter</t>
   </si>
   <si>
-    <t>Poulter, Ian</t>
-  </si>
-  <si>
-    <t>Hahn, James</t>
-  </si>
-  <si>
     <t>Levy, Alexander</t>
   </si>
   <si>
     <t>Howell III, Charles</t>
   </si>
   <si>
+    <t>Na, Kevin</t>
+  </si>
+  <si>
+    <t>Moore, Ryan</t>
+  </si>
+  <si>
+    <t>Snedeker, Brandt</t>
+  </si>
+  <si>
+    <t>Luiten, Joost</t>
+  </si>
+  <si>
     <t>Bradley, Keegan</t>
   </si>
   <si>
     <t>Suri, Julian</t>
   </si>
   <si>
-    <t>Snedeker, Brandt</t>
-  </si>
-  <si>
     <t>Haas, Bill</t>
   </si>
   <si>
@@ -233,9 +245,6 @@
     <t>Lowry, Shane</t>
   </si>
   <si>
-    <t>Moore, Ryan</t>
-  </si>
-  <si>
     <t>Sharma, Shubhankar</t>
   </si>
   <si>
@@ -245,70 +254,73 @@
     <t>Potter Jr, Ted</t>
   </si>
   <si>
+    <t>Lahiri, Anirban</t>
+  </si>
+  <si>
     <t>Westwood, Lee</t>
   </si>
   <si>
+    <t>Schniederjans, Ollie</t>
+  </si>
+  <si>
+    <t>Bryan, Wesley</t>
+  </si>
+  <si>
     <t>Horschel, Billy</t>
   </si>
   <si>
-    <t>Bryan, Wesley</t>
-  </si>
-  <si>
-    <t>Lahiri, Anirban</t>
-  </si>
-  <si>
     <t>Kaymer, Martin</t>
   </si>
   <si>
-    <t>Schniederjans, Ollie</t>
-  </si>
-  <si>
     <t>Dunne, Paul</t>
   </si>
   <si>
+    <t>Paisley, Chris</t>
+  </si>
+  <si>
+    <t>Han, Seungsu</t>
+  </si>
+  <si>
     <t>Grillo, Emiliano</t>
   </si>
   <si>
     <t>Walker, Jimmy</t>
   </si>
   <si>
-    <t>Paisley, Chris</t>
-  </si>
-  <si>
     <t>Holmes, J.B.</t>
   </si>
   <si>
     <t>Knox, Russell</t>
   </si>
   <si>
+    <t>Wood, Chris</t>
+  </si>
+  <si>
+    <t>Kang, Sunghoon</t>
+  </si>
+  <si>
     <t>Olesen, Thorbjorn</t>
   </si>
   <si>
+    <t>DeChambeau, Bryson</t>
+  </si>
+  <si>
     <t>Kim, Chan</t>
   </si>
   <si>
-    <t>Han, Seungsu</t>
-  </si>
-  <si>
-    <t>DeChambeau, Bryson</t>
-  </si>
-  <si>
-    <t>Luiten, Joost</t>
-  </si>
-  <si>
-    <t>Kang, Sunghoon</t>
+    <t>Zanotti, Fabrizio</t>
   </si>
   <si>
     <t>Glover, Lucas</t>
   </si>
   <si>
+    <t>Imahira, Shugo</t>
+  </si>
+  <si>
     <t>Hun An, Byeong</t>
   </si>
   <si>
-    <t>Imahira, Shugo</t>
-  </si>
-  <si>
-    <t>Na, Kevin</t>
+    <t>Palmer, Ryan</t>
   </si>
   <si>
     <t>Dubuisson, Victor</t>
@@ -317,15 +329,9 @@
     <t>Fox, Ryan</t>
   </si>
   <si>
-    <t>Palmer, Ryan</t>
-  </si>
-  <si>
     <t>Swafford, Hudson</t>
   </si>
   <si>
-    <t>Zanotti, Fabrizio</t>
-  </si>
-  <si>
     <t>Im, Sungjae</t>
   </si>
   <si>
@@ -386,16 +392,10 @@
     <t>Wang, Jeunghun</t>
   </si>
   <si>
-    <t>Watson, Bubba</t>
-  </si>
-  <si>
     <t>Westwoon, Lee</t>
   </si>
   <si>
     <t>Willett, Danny</t>
-  </si>
-  <si>
-    <t>Wood, Chris</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -1009,7 +1009,7 @@
       <c r="C25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="3" t="n"/>
+      <c r="D25" s="4" t="n"/>
     </row>
     <row r="26" spans="1:5">
       <c r="B26" s="1" t="n">
@@ -1036,7 +1036,7 @@
       <c r="C28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="4" t="n"/>
+      <c r="D28" s="3" t="n"/>
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="1" t="n">
@@ -1117,7 +1117,7 @@
       <c r="C37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="3" t="n"/>
+      <c r="D37" s="4" t="n"/>
     </row>
     <row r="38" spans="1:5">
       <c r="B38" s="1" t="n">
@@ -1153,7 +1153,7 @@
       <c r="C41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="3" t="n"/>
+      <c r="D41" s="4" t="n"/>
     </row>
     <row r="42" spans="1:5">
       <c r="B42" s="1" t="n">
@@ -1162,7 +1162,7 @@
       <c r="C42" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="4" t="n"/>
+      <c r="D42" s="3" t="n"/>
     </row>
     <row r="43" spans="1:5">
       <c r="B43" s="1" t="n">
@@ -1171,7 +1171,7 @@
       <c r="C43" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="4" t="n"/>
+      <c r="D43" s="3" t="n"/>
     </row>
     <row r="44" spans="1:5">
       <c r="B44" s="1" t="n">
@@ -1234,7 +1234,7 @@
       <c r="C50" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D50" s="3" t="n"/>
+      <c r="D50" s="4" t="n"/>
     </row>
     <row r="51" spans="1:5">
       <c r="B51" s="1" t="n">
@@ -1243,7 +1243,7 @@
       <c r="C51" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D51" s="4" t="n"/>
+      <c r="D51" s="3" t="n"/>
     </row>
     <row r="52" spans="1:5">
       <c r="B52" s="1" t="n">
@@ -1252,7 +1252,7 @@
       <c r="C52" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="4" t="n"/>
+      <c r="D52" s="3" t="n"/>
     </row>
     <row r="53" spans="1:5">
       <c r="B53" s="1" t="n">
@@ -1288,7 +1288,7 @@
       <c r="C56" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D56" s="4" t="n"/>
+      <c r="D56" s="3" t="n"/>
     </row>
     <row r="57" spans="1:5">
       <c r="B57" s="1" t="n">
@@ -1306,7 +1306,7 @@
       <c r="C58" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D58" s="3" t="n"/>
+      <c r="D58" s="4" t="n"/>
     </row>
     <row r="59" spans="1:5">
       <c r="B59" s="1" t="n">
@@ -1324,7 +1324,7 @@
       <c r="C60" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D60" s="3" t="n"/>
+      <c r="D60" s="4" t="n"/>
     </row>
     <row r="61" spans="1:5">
       <c r="B61" s="1" t="n">
@@ -1342,7 +1342,7 @@
       <c r="C62" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D62" s="4" t="n"/>
+      <c r="D62" s="3" t="n"/>
     </row>
     <row r="63" spans="1:5">
       <c r="B63" s="1" t="n">
@@ -1378,7 +1378,7 @@
       <c r="C66" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D66" s="3" t="n"/>
+      <c r="D66" s="4" t="n"/>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="5" t="n"/>
@@ -1398,7 +1398,7 @@
       <c r="C68" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D68" s="4" t="n"/>
+      <c r="D68" s="3" t="n"/>
     </row>
     <row r="69" spans="1:5">
       <c r="B69" s="1" t="n">
@@ -1425,7 +1425,7 @@
       <c r="C71" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D71" s="4" t="n"/>
+      <c r="D71" s="3" t="n"/>
     </row>
     <row r="72" spans="1:5">
       <c r="B72" s="1" t="n">
@@ -1434,7 +1434,7 @@
       <c r="C72" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D72" s="3" t="n"/>
+      <c r="D72" s="4" t="n"/>
     </row>
     <row r="73" spans="1:5">
       <c r="B73" s="1" t="n">
@@ -1443,7 +1443,7 @@
       <c r="C73" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D73" s="3" t="n"/>
+      <c r="D73" s="4" t="n"/>
     </row>
     <row r="74" spans="1:5">
       <c r="B74" s="1" t="n">
@@ -1452,7 +1452,7 @@
       <c r="C74" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D74" s="4" t="n"/>
+      <c r="D74" s="3" t="n"/>
     </row>
     <row r="75" spans="1:5">
       <c r="B75" s="1" t="n">
@@ -1461,7 +1461,7 @@
       <c r="C75" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D75" s="3" t="n"/>
+      <c r="D75" s="4" t="n"/>
     </row>
     <row r="76" spans="1:5">
       <c r="B76" s="1" t="n">
@@ -1470,7 +1470,7 @@
       <c r="C76" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D76" s="4" t="n"/>
+      <c r="D76" s="3" t="n"/>
     </row>
     <row r="77" spans="1:5">
       <c r="B77" s="1" t="n">
@@ -1479,7 +1479,7 @@
       <c r="C77" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D77" s="3" t="n"/>
+      <c r="D77" s="4" t="n"/>
     </row>
     <row r="78" spans="1:5">
       <c r="B78" s="1" t="n">
@@ -1569,7 +1569,7 @@
       <c r="C87" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D87" s="3" t="n"/>
+      <c r="D87" s="4" t="n"/>
     </row>
     <row r="88" spans="1:5">
       <c r="B88" s="1" t="n">
@@ -1578,7 +1578,7 @@
       <c r="C88" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D88" s="3" t="n"/>
+      <c r="D88" s="4" t="n"/>
     </row>
     <row r="89" spans="1:5">
       <c r="B89" s="1" t="n">
@@ -1587,7 +1587,7 @@
       <c r="C89" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D89" s="4" t="n"/>
+      <c r="D89" s="3" t="n"/>
     </row>
     <row r="90" spans="1:5">
       <c r="B90" s="1" t="n">
@@ -1596,7 +1596,7 @@
       <c r="C90" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D90" s="4" t="n"/>
+      <c r="D90" s="3" t="n"/>
     </row>
     <row r="91" spans="1:5">
       <c r="B91" s="1" t="n">
@@ -1605,7 +1605,7 @@
       <c r="C91" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D91" s="4" t="n"/>
+      <c r="D91" s="3" t="n"/>
     </row>
     <row r="92" spans="1:5">
       <c r="B92" s="1" t="n">
@@ -1614,7 +1614,7 @@
       <c r="C92" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D92" s="4" t="n"/>
+      <c r="D92" s="3" t="n"/>
     </row>
     <row r="93" spans="1:5">
       <c r="B93" s="1" t="n">
@@ -1650,7 +1650,7 @@
       <c r="C96" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D96" s="3" t="n"/>
+      <c r="D96" s="4" t="n"/>
     </row>
     <row r="97" spans="1:5">
       <c r="B97" s="1" t="n">
@@ -1668,7 +1668,7 @@
       <c r="C98" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D98" s="3" t="n"/>
+      <c r="D98" s="4" t="n"/>
     </row>
     <row r="99" spans="1:5">
       <c r="B99" s="1" t="n">
@@ -1695,7 +1695,7 @@
       <c r="C101" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D101" s="4" t="n"/>
+      <c r="D101" s="3" t="n"/>
     </row>
     <row r="102" spans="1:5">
       <c r="B102" s="1" t="n">
@@ -1740,7 +1740,7 @@
       <c r="C106" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D106" s="3" t="n"/>
+      <c r="D106" s="4" t="n"/>
     </row>
     <row r="107" spans="1:5">
       <c r="B107" s="1" t="n">
@@ -1749,7 +1749,7 @@
       <c r="C107" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D107" s="3" t="n"/>
+      <c r="D107" s="4" t="n"/>
     </row>
     <row r="108" spans="1:5">
       <c r="B108" s="1" t="n">

</xml_diff>

<commit_message>
updates Excel file with cy's new photography
</commit_message>
<xml_diff>
--- a/OWGR.xlsx
+++ b/OWGR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28421"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="2180" windowWidth="25600" windowHeight="15620"/>
+    <workbookView xWindow="5240" yWindow="6980" windowWidth="25600" windowHeight="15620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -816,7 +816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
       <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Rebuild using py2app. Changes reflect main app rename from 8_*.py to OWGR.py
</commit_message>
<xml_diff>
--- a/OWGR.xlsx
+++ b/OWGR.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28421"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="5240" yWindow="6980" windowWidth="25600" windowHeight="15620"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134">
   <si>
     <t>RANK</t>
   </si>
@@ -39,12 +35,12 @@
     <t>Rahm, Jon</t>
   </si>
   <si>
+    <t>Thomas, Justin</t>
+  </si>
+  <si>
     <t>Spieth, Jordan</t>
   </si>
   <si>
-    <t>Thomas, Justin</t>
-  </si>
-  <si>
     <t>Rose, Justin</t>
   </si>
   <si>
@@ -63,22 +59,25 @@
     <t>McIlroy, Rory</t>
   </si>
   <si>
+    <t>Fleetwood, Tommy</t>
+  </si>
+  <si>
     <t>Garcia, Sergio</t>
   </si>
   <si>
-    <t>Fleetwood, Tommy</t>
-  </si>
-  <si>
     <t>Stenson, Henrik</t>
   </si>
   <si>
+    <t>Noren, Alex</t>
+  </si>
+  <si>
     <t>Leishman, Marc</t>
   </si>
   <si>
     <t>Hatton, Tyrrell</t>
   </si>
   <si>
-    <t>Noren, Alex</t>
+    <t>Casey, Paul</t>
   </si>
   <si>
     <t>Kuchar, Matt</t>
@@ -87,30 +86,27 @@
     <t>Perez, Pat</t>
   </si>
   <si>
-    <t>Casey, Paul</t>
-  </si>
-  <si>
     <t>Cabrera Bello, Rafael</t>
   </si>
   <si>
     <t>Harman, Brian</t>
   </si>
   <si>
+    <t>Molinari, Francesco</t>
+  </si>
+  <si>
     <t>Schauffele, Xander</t>
   </si>
   <si>
     <t>Hoffman, Charley</t>
   </si>
   <si>
-    <t>Molinari, Francesco</t>
+    <t>Woodland, Gary</t>
   </si>
   <si>
     <t>Reed, Patrick</t>
   </si>
   <si>
-    <t>Woodland, Gary</t>
-  </si>
-  <si>
     <t>Fisher, Ross</t>
   </si>
   <si>
@@ -126,28 +122,34 @@
     <t>Kisner, Kevin</t>
   </si>
   <si>
+    <t>Finau, Tony</t>
+  </si>
+  <si>
+    <t>Berger, Daniel</t>
+  </si>
+  <si>
     <t>Mickelson, Phil</t>
   </si>
   <si>
-    <t>Finau, Tony</t>
-  </si>
-  <si>
     <t>Cantlay, Patrick</t>
   </si>
   <si>
-    <t>Berger, Daniel</t>
-  </si>
-  <si>
     <t>Chappell, Kevin</t>
   </si>
   <si>
     <t>Haotong, Li</t>
   </si>
   <si>
+    <t>Steele, Brendan</t>
+  </si>
+  <si>
+    <t>Pieters, Thomas</t>
+  </si>
+  <si>
     <t>Aphibarnrat, Kiradech</t>
   </si>
   <si>
-    <t>Steele, Brendan</t>
+    <t>Simpson, Webb</t>
   </si>
   <si>
     <t>Watson, Bubba</t>
@@ -156,33 +158,27 @@
     <t>Kodaira, Satoshi</t>
   </si>
   <si>
-    <t>Pieters, Thomas</t>
+    <t>Frittelli, Dylan</t>
+  </si>
+  <si>
+    <t>Dufner, Jason</t>
   </si>
   <si>
     <t>Reavie, Chez</t>
   </si>
   <si>
-    <t>Dufner, Jason</t>
-  </si>
-  <si>
-    <t>Simpson, Webb</t>
+    <t>Schwartzel, Charl</t>
   </si>
   <si>
     <t>Ikeda, Yuta</t>
   </si>
   <si>
-    <t>Frittelli, Dylan</t>
-  </si>
-  <si>
-    <t>Schwartzel, Charl</t>
+    <t>Hadwin, Adam</t>
   </si>
   <si>
     <t>Vegas, Jhonattan</t>
   </si>
   <si>
-    <t>Hadwin, Adam</t>
-  </si>
-  <si>
     <t>Kim, Siwoo</t>
   </si>
   <si>
@@ -198,30 +194,30 @@
     <t>Henley, Russell</t>
   </si>
   <si>
+    <t>Scott, Adam</t>
+  </si>
+  <si>
     <t>Stanley, Kyle</t>
   </si>
   <si>
     <t>Hahn, James</t>
   </si>
   <si>
-    <t>Scott, Adam</t>
+    <t>Kizzire, Patton</t>
   </si>
   <si>
     <t>Johnson, Zach</t>
   </si>
   <si>
-    <t>Kizzire, Patton</t>
+    <t>Levy, Alexander</t>
+  </si>
+  <si>
+    <t>Uihlein, Peter</t>
   </si>
   <si>
     <t>Poulter, Ian</t>
   </si>
   <si>
-    <t>Uihlein, Peter</t>
-  </si>
-  <si>
-    <t>Levy, Alexander</t>
-  </si>
-  <si>
     <t>Howell III, Charles</t>
   </si>
   <si>
@@ -231,22 +227,25 @@
     <t>Moore, Ryan</t>
   </si>
   <si>
+    <t>Luiten, Joost</t>
+  </si>
+  <si>
+    <t>Bradley, Keegan</t>
+  </si>
+  <si>
+    <t>Haas, Bill</t>
+  </si>
+  <si>
+    <t>Suri, Julian</t>
+  </si>
+  <si>
+    <t>Hadley, Chesson</t>
+  </si>
+  <si>
     <t>Snedeker, Brandt</t>
   </si>
   <si>
-    <t>Luiten, Joost</t>
-  </si>
-  <si>
-    <t>Bradley, Keegan</t>
-  </si>
-  <si>
-    <t>Suri, Julian</t>
-  </si>
-  <si>
-    <t>Haas, Bill</t>
-  </si>
-  <si>
-    <t>Hadley, Chesson</t>
+    <t>List, Luke</t>
   </si>
   <si>
     <t>Lowry, Shane</t>
@@ -255,6 +254,9 @@
     <t>Sharma, Shubhankar</t>
   </si>
   <si>
+    <t>Grillo, Emiliano</t>
+  </si>
+  <si>
     <t>Tanihara, Hideto</t>
   </si>
   <si>
@@ -270,63 +272,66 @@
     <t>Schniederjans, Ollie</t>
   </si>
   <si>
+    <t>Han, Seungsu</t>
+  </si>
+  <si>
+    <t>Paisley, Chris</t>
+  </si>
+  <si>
+    <t>Hun An, Byeong</t>
+  </si>
+  <si>
     <t>Bryan, Wesley</t>
   </si>
   <si>
+    <t>Dunne, Paul</t>
+  </si>
+  <si>
     <t>Horschel, Billy</t>
   </si>
   <si>
     <t>Kaymer, Martin</t>
   </si>
   <si>
-    <t>Dunne, Paul</t>
-  </si>
-  <si>
-    <t>Paisley, Chris</t>
-  </si>
-  <si>
-    <t>Han, Seungsu</t>
-  </si>
-  <si>
-    <t>Grillo, Emiliano</t>
-  </si>
-  <si>
     <t>Walker, Jimmy</t>
   </si>
   <si>
     <t>Holmes, J.B.</t>
   </si>
   <si>
+    <t>Wood, Chris</t>
+  </si>
+  <si>
+    <t>Pepperell, Eddie</t>
+  </si>
+  <si>
+    <t>Kang, Sunghoon</t>
+  </si>
+  <si>
     <t>Knox, Russell</t>
   </si>
   <si>
-    <t>Wood, Chris</t>
-  </si>
-  <si>
-    <t>Kang, Sunghoon</t>
+    <t>DeChambeau, Bryson</t>
   </si>
   <si>
     <t>Olesen, Thorbjorn</t>
   </si>
   <si>
-    <t>DeChambeau, Bryson</t>
-  </si>
-  <si>
     <t>Kim, Chan</t>
   </si>
   <si>
+    <t>Lovemark, Jamie</t>
+  </si>
+  <si>
+    <t>Glover, Lucas</t>
+  </si>
+  <si>
     <t>Zanotti, Fabrizio</t>
   </si>
   <si>
-    <t>Glover, Lucas</t>
-  </si>
-  <si>
     <t>Imahira, Shugo</t>
   </si>
   <si>
-    <t>Hun An, Byeong</t>
-  </si>
-  <si>
     <t>Palmer, Ryan</t>
   </si>
   <si>
@@ -346,9 +351,6 @@
   </si>
   <si>
     <t>An, Byuonghun</t>
-  </si>
-  <si>
-    <t>Cabrea bello, Rafa</t>
   </si>
   <si>
     <t>Castro, Roberto</t>
@@ -420,24 +422,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="14"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -464,68 +466,60 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left style="thin"/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thick"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="10">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf borderId="2" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:E131">
-  <autoFilter ref="B3:E131"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table1" headerRowCount="1" id="1" name="Table1" ref="B3:E133">
+  <autoFilter ref="B3:E133"/>
   <tableColumns count="4">
     <tableColumn id="2" name="RANK"/>
     <tableColumn id="3" name="Player Name"/>
     <tableColumn id="4" name="2017"/>
     <tableColumn id="5" name="2018"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight8" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="0"/>
 </table>
 </file>
 
@@ -813,21 +807,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F131"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A3:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="5" width="10" customWidth="1"/>
+    <col customWidth="1" max="2" min="2" width="6"/>
+    <col customWidth="1" max="3" min="3" width="20"/>
+    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="5" min="5" width="10"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -841,1297 +840,1312 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="18">
-      <c r="B4" s="1">
+    <row r="4" spans="1:6">
+      <c r="B4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="2:5" ht="18">
-      <c r="B5" s="1">
+      <c r="D4" s="3" t="n"/>
+      <c r="E4" s="4" t="n"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="2:5" ht="18">
-      <c r="B6" s="1">
+      <c r="D5" s="3" t="n"/>
+      <c r="E5" s="4" t="n"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="2:5" ht="18">
-      <c r="B7" s="1">
+      <c r="D6" s="3" t="n"/>
+      <c r="E6" s="4" t="n"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="2:5" ht="18">
-      <c r="B8" s="1">
+      <c r="D7" s="3" t="n"/>
+      <c r="E7" s="4" t="n"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="2:5" ht="18">
-      <c r="B9" s="1">
+      <c r="D8" s="3" t="n"/>
+      <c r="E8" s="4" t="n"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="2:5" ht="18">
-      <c r="B10" s="1">
+      <c r="D9" s="3" t="n"/>
+      <c r="E9" s="4" t="n"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" s="1" t="n">
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="2:5" ht="18">
-      <c r="B11" s="1">
+      <c r="D10" s="3" t="n"/>
+      <c r="E10" s="4" t="n"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" s="1" t="n">
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="2:5" ht="18">
-      <c r="B12" s="1">
+      <c r="D11" s="3" t="n"/>
+      <c r="E11" s="4" t="n"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" s="1" t="n">
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="2:5" ht="18">
-      <c r="B13" s="1">
+      <c r="D12" s="3" t="n"/>
+      <c r="E12" s="4" t="n"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="1" t="n">
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="2:5" ht="18">
-      <c r="B14" s="1">
+      <c r="D13" s="3" t="n"/>
+      <c r="E13" s="4" t="n"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="1" t="n">
         <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="2:5" ht="18">
-      <c r="B15" s="1">
+      <c r="D14" s="3" t="n"/>
+      <c r="E14" s="4" t="n"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" s="1" t="n">
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="2:5" ht="18">
-      <c r="B16" s="1">
+      <c r="D15" s="3" t="n"/>
+      <c r="E15" s="3" t="n"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" s="1" t="n">
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="2:5" ht="18">
-      <c r="B17" s="1">
+      <c r="D16" s="3" t="n"/>
+      <c r="E16" s="4" t="n"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="B17" s="1" t="n">
         <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="2:5" ht="18">
-      <c r="B18" s="1">
+      <c r="D17" s="3" t="n"/>
+      <c r="E17" s="3" t="n"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="B18" s="1" t="n">
         <v>15</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="2:5" ht="18">
-      <c r="B19" s="1">
+      <c r="D18" s="3" t="n"/>
+      <c r="E18" s="4" t="n"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="B19" s="1" t="n">
         <v>16</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="2:5" ht="18">
-      <c r="B20" s="1">
+      <c r="D19" s="4" t="n"/>
+      <c r="E19" s="3" t="n"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="B20" s="1" t="n">
         <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="2:5" ht="18">
-      <c r="B21" s="1">
+      <c r="D20" s="3" t="n"/>
+      <c r="E20" s="4" t="n"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="B21" s="1" t="n">
         <v>18</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="2:5" ht="18">
-      <c r="B22" s="1">
+      <c r="D21" s="3" t="n"/>
+      <c r="E21" s="4" t="n"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22" s="1" t="n">
         <v>19</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="2:5" ht="18">
-      <c r="B23" s="1">
+      <c r="D22" s="3" t="n"/>
+      <c r="E22" s="4" t="n"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="B23" s="1" t="n">
         <v>20</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="2:5" ht="18">
-      <c r="B24" s="1">
+      <c r="D23" s="3" t="n"/>
+      <c r="E23" s="3" t="n"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="B24" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="2:5" ht="18">
-      <c r="B25" s="1">
+      <c r="D24" s="4" t="n"/>
+      <c r="E24" s="4" t="n"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="B25" s="1" t="n">
         <v>22</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="2:5" ht="18">
-      <c r="B26" s="1">
+      <c r="D25" s="3" t="n"/>
+      <c r="E25" s="4" t="n"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="B26" s="1" t="n">
         <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="2:5" ht="18">
-      <c r="B27" s="1">
+      <c r="D26" s="4" t="n"/>
+      <c r="E26" s="4" t="n"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="B27" s="1" t="n">
         <v>24</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="2:5" ht="18">
-      <c r="B28" s="1">
+      <c r="D27" s="4" t="n"/>
+      <c r="E27" s="4" t="n"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="B28" s="1" t="n">
         <v>25</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="2:5" ht="18">
-      <c r="B29" s="1">
+      <c r="D28" s="3" t="n"/>
+      <c r="E28" s="3" t="n"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="B29" s="1" t="n">
         <v>26</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="2:5" ht="18">
-      <c r="B30" s="1">
+      <c r="D29" s="3" t="n"/>
+      <c r="E29" s="4" t="n"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="B30" s="1" t="n">
         <v>27</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="2:5" ht="18">
-      <c r="B31" s="1">
+      <c r="D30" s="3" t="n"/>
+      <c r="E30" s="4" t="n"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="B31" s="1" t="n">
         <v>28</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="2:5" ht="18">
-      <c r="B32" s="1">
+      <c r="D31" s="3" t="n"/>
+      <c r="E31" s="4" t="n"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="B32" s="1" t="n">
         <v>29</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="2:5" ht="18">
-      <c r="B33" s="1">
+      <c r="D32" s="3" t="n"/>
+      <c r="E32" s="3" t="n"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="2:5" ht="18">
-      <c r="B34" s="1">
+      <c r="D33" s="4" t="n"/>
+      <c r="E33" s="4" t="n"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34" s="1" t="n">
         <v>31</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="2:5" ht="18">
-      <c r="B35" s="1">
+      <c r="D34" s="3" t="n"/>
+      <c r="E34" s="4" t="n"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" s="1" t="n">
         <v>32</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="2:5" ht="18">
-      <c r="B36" s="1">
+      <c r="D35" s="4" t="n"/>
+      <c r="E35" s="4" t="n"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36" s="1" t="n">
         <v>33</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="2:5" ht="18">
-      <c r="B37" s="1">
+      <c r="D36" s="3" t="n"/>
+      <c r="E36" s="4" t="n"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37" s="1" t="n">
         <v>34</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="2:5" ht="18">
-      <c r="B38" s="1">
+      <c r="D37" s="3" t="n"/>
+      <c r="E37" s="4" t="n"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="B38" s="1" t="n">
         <v>35</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="2:5" ht="18">
-      <c r="B39" s="1">
+      <c r="D38" s="4" t="n"/>
+      <c r="E38" s="4" t="n"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="B39" s="1" t="n">
         <v>36</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="2:5" ht="18">
-      <c r="B40" s="1">
+      <c r="D39" s="3" t="n"/>
+      <c r="E39" s="4" t="n"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="B40" s="1" t="n">
         <v>37</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-    </row>
-    <row r="41" spans="2:5" ht="18">
-      <c r="B41" s="1">
+      <c r="D40" s="4" t="n"/>
+      <c r="E40" s="4" t="n"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="B41" s="1" t="n">
         <v>38</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="2:5" ht="18">
-      <c r="B42" s="1">
+      <c r="D41" s="3" t="n"/>
+      <c r="E41" s="4" t="n"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="B42" s="1" t="n">
         <v>39</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="2:5" ht="18">
-      <c r="B43" s="1">
+      <c r="D42" s="3" t="n"/>
+      <c r="E42" s="4" t="n"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="B43" s="1" t="n">
         <v>40</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="2:5" ht="18">
-      <c r="B44" s="1">
+      <c r="D43" s="4" t="n"/>
+      <c r="E43" s="4" t="n"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="B44" s="1" t="n">
         <v>41</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-    </row>
-    <row r="45" spans="2:5" ht="18">
-      <c r="B45" s="1">
-        <v>42</v>
+      <c r="D44" s="3" t="n"/>
+      <c r="E44" s="3" t="n"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="B45" s="1" t="n">
+        <v>41</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="4"/>
-    </row>
-    <row r="46" spans="2:5" ht="18">
-      <c r="B46" s="1">
+      <c r="D45" s="3" t="n"/>
+      <c r="E45" s="4" t="n"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="B46" s="1" t="n">
         <v>43</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" spans="2:5" ht="18">
-      <c r="B47" s="1">
+      <c r="D46" s="4" t="n"/>
+      <c r="E46" s="4" t="n"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="B47" s="1" t="n">
         <v>44</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" spans="2:5" ht="18">
-      <c r="B48" s="1">
+      <c r="D47" s="4" t="n"/>
+      <c r="E47" s="4" t="n"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="B48" s="1" t="n">
         <v>45</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="2:5" ht="18">
-      <c r="B49" s="1">
+      <c r="D48" s="3" t="n"/>
+      <c r="E48" s="4" t="n"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="B49" s="1" t="n">
         <v>46</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="4"/>
-    </row>
-    <row r="50" spans="2:5" ht="18">
-      <c r="B50" s="1">
+      <c r="D49" s="4" t="n"/>
+      <c r="E49" s="4" t="n"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="B50" s="1" t="n">
         <v>47</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-    </row>
-    <row r="51" spans="2:5" ht="18">
-      <c r="B51" s="1">
+      <c r="D50" s="3" t="n"/>
+      <c r="E50" s="4" t="n"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="B51" s="1" t="n">
         <v>48</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="4"/>
-    </row>
-    <row r="52" spans="2:5" ht="18">
-      <c r="B52" s="1">
+      <c r="D51" s="3" t="n"/>
+      <c r="E51" s="4" t="n"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="B52" s="1" t="n">
         <v>49</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="4"/>
-    </row>
-    <row r="53" spans="2:5" ht="18">
-      <c r="B53" s="1">
+      <c r="D52" s="3" t="n"/>
+      <c r="E52" s="4" t="n"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="B53" s="1" t="n">
         <v>50</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="4"/>
-    </row>
-    <row r="54" spans="2:5" ht="18">
-      <c r="B54" s="1">
+      <c r="D53" s="3" t="n"/>
+      <c r="E53" s="4" t="n"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="B54" s="1" t="n">
         <v>51</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-    </row>
-    <row r="55" spans="2:5" ht="18">
-      <c r="B55" s="1">
+      <c r="D54" s="4" t="n"/>
+      <c r="E54" s="4" t="n"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="B55" s="1" t="n">
         <v>52</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-    </row>
-    <row r="56" spans="2:5" ht="18">
-      <c r="B56" s="1">
+      <c r="D55" s="4" t="n"/>
+      <c r="E55" s="4" t="n"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="B56" s="1" t="n">
         <v>53</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D56" s="3"/>
-      <c r="E56" s="4"/>
-    </row>
-    <row r="57" spans="2:5" ht="18">
-      <c r="B57" s="1">
+      <c r="D56" s="3" t="n"/>
+      <c r="E56" s="4" t="n"/>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="B57" s="1" t="n">
         <v>54</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-    </row>
-    <row r="58" spans="2:5" ht="18">
-      <c r="B58" s="1">
+      <c r="D57" s="4" t="n"/>
+      <c r="E57" s="4" t="n"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="B58" s="1" t="n">
         <v>55</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D58" s="4"/>
-      <c r="E58" s="3"/>
-    </row>
-    <row r="59" spans="2:5" ht="18">
-      <c r="B59" s="1">
+      <c r="D58" s="4" t="n"/>
+      <c r="E58" s="3" t="n"/>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="B59" s="1" t="n">
         <v>56</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-    </row>
-    <row r="60" spans="2:5" ht="18">
-      <c r="B60" s="1">
+      <c r="D59" s="4" t="n"/>
+      <c r="E59" s="4" t="n"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="B60" s="1" t="n">
         <v>57</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-    </row>
-    <row r="61" spans="2:5" ht="18">
-      <c r="B61" s="1">
+      <c r="D60" s="4" t="n"/>
+      <c r="E60" s="4" t="n"/>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="B61" s="1" t="n">
         <v>58</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-    </row>
-    <row r="62" spans="2:5" ht="18">
-      <c r="B62" s="1">
+      <c r="D61" s="4" t="n"/>
+      <c r="E61" s="4" t="n"/>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="B62" s="1" t="n">
         <v>59</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D62" s="3"/>
-      <c r="E62" s="4"/>
-    </row>
-    <row r="63" spans="2:5" ht="18">
-      <c r="B63" s="1">
+      <c r="D62" s="4" t="n"/>
+      <c r="E62" s="3" t="n"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="B63" s="1" t="n">
         <v>60</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D63" s="4"/>
-      <c r="E63" s="3"/>
-    </row>
-    <row r="64" spans="2:5" ht="18">
-      <c r="B64" s="1">
+      <c r="D63" s="3" t="n"/>
+      <c r="E63" s="4" t="n"/>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="B64" s="1" t="n">
         <v>61</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D64" s="4"/>
-      <c r="E64" s="3"/>
-    </row>
-    <row r="65" spans="1:6" ht="18">
-      <c r="B65" s="1">
+      <c r="D64" s="4" t="n"/>
+      <c r="E64" s="4" t="n"/>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="B65" s="1" t="n">
         <v>62</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-    </row>
-    <row r="66" spans="1:6" ht="18">
-      <c r="B66" s="1">
+      <c r="D65" s="4" t="n"/>
+      <c r="E65" s="4" t="n"/>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="B66" s="1" t="n">
         <v>63</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-    </row>
-    <row r="67" spans="1:6" ht="18">
-      <c r="A67" s="5"/>
-      <c r="B67" s="6">
+      <c r="D66" s="4" t="n"/>
+      <c r="E66" s="3" t="n"/>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="5" t="n"/>
+      <c r="B67" s="6" t="n">
         <v>64</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D67" s="8"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="5"/>
-    </row>
-    <row r="68" spans="1:6" ht="18">
-      <c r="B68" s="1">
+      <c r="D67" s="8" t="n"/>
+      <c r="E67" s="9" t="n"/>
+      <c r="F67" s="5" t="n"/>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="B68" s="1" t="n">
         <v>65</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D68" s="3"/>
-      <c r="E68" s="4"/>
-    </row>
-    <row r="69" spans="1:6" ht="18">
-      <c r="B69" s="1">
+      <c r="D68" s="3" t="n"/>
+      <c r="E68" s="4" t="n"/>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="B69" s="1" t="n">
         <v>66</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D69" s="3"/>
-      <c r="E69" s="4"/>
-    </row>
-    <row r="70" spans="1:6" ht="18">
-      <c r="B70" s="1">
+      <c r="D69" s="3" t="n"/>
+      <c r="E69" s="4" t="n"/>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="B70" s="1" t="n">
         <v>67</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-    </row>
-    <row r="71" spans="1:6" ht="18">
-      <c r="B71" s="1">
+      <c r="D70" s="3" t="n"/>
+      <c r="E70" s="4" t="n"/>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="B71" s="1" t="n">
         <v>68</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D71" s="3"/>
-      <c r="E71" s="4"/>
-    </row>
-    <row r="72" spans="1:6" ht="18">
-      <c r="B72" s="1">
+      <c r="D71" s="4" t="n"/>
+      <c r="E71" s="4" t="n"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="B72" s="1" t="n">
         <v>69</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
-    </row>
-    <row r="73" spans="1:6" ht="18">
-      <c r="B73" s="1">
+      <c r="D72" s="3" t="n"/>
+      <c r="E72" s="4" t="n"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="B73" s="1" t="n">
         <v>70</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
-    </row>
-    <row r="74" spans="1:6" ht="18">
-      <c r="B74" s="1">
+      <c r="D73" s="4" t="n"/>
+      <c r="E73" s="4" t="n"/>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="B74" s="1" t="n">
         <v>71</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D74" s="3"/>
-      <c r="E74" s="4"/>
-    </row>
-    <row r="75" spans="1:6" ht="18">
-      <c r="B75" s="1">
+      <c r="D74" s="4" t="n"/>
+      <c r="E74" s="3" t="n"/>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="B75" s="1" t="n">
         <v>72</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D75" s="4"/>
-      <c r="E75" s="3"/>
-    </row>
-    <row r="76" spans="1:6" ht="18">
-      <c r="B76" s="1">
+      <c r="D75" s="3" t="n"/>
+      <c r="E75" s="3" t="n"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="B76" s="1" t="n">
         <v>73</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-    </row>
-    <row r="77" spans="1:6" ht="18">
-      <c r="B77" s="1">
+      <c r="D76" s="4" t="n"/>
+      <c r="E76" s="4" t="n"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="B77" s="1" t="n">
         <v>74</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
-    </row>
-    <row r="78" spans="1:6" ht="18">
-      <c r="B78" s="1">
+      <c r="D77" s="3" t="n"/>
+      <c r="E77" s="3" t="n"/>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="B78" s="1" t="n">
         <v>75</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D78" s="3"/>
-      <c r="E78" s="4"/>
-    </row>
-    <row r="79" spans="1:6" ht="18">
-      <c r="B79" s="1">
+      <c r="D78" s="4" t="n"/>
+      <c r="E78" s="4" t="n"/>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="B79" s="1" t="n">
         <v>76</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D79" s="4"/>
-      <c r="E79" s="3"/>
-    </row>
-    <row r="80" spans="1:6" ht="18">
-      <c r="B80" s="1">
+      <c r="D79" s="3" t="n"/>
+      <c r="E79" s="4" t="n"/>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="B80" s="1" t="n">
         <v>77</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
-    </row>
-    <row r="81" spans="2:5" ht="18">
-      <c r="B81" s="1">
+      <c r="D80" s="3" t="n"/>
+      <c r="E80" s="4" t="n"/>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="B81" s="1" t="n">
         <v>78</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D81" s="3"/>
-      <c r="E81" s="4"/>
-    </row>
-    <row r="82" spans="2:5" ht="18">
-      <c r="B82" s="1">
+      <c r="D81" s="4" t="n"/>
+      <c r="E81" s="3" t="n"/>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="B82" s="1" t="n">
         <v>79</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D82" s="4"/>
-      <c r="E82" s="3"/>
-    </row>
-    <row r="83" spans="2:5" ht="18">
-      <c r="B83" s="1">
+      <c r="D82" s="4" t="n"/>
+      <c r="E82" s="4" t="n"/>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="B83" s="1" t="n">
         <v>80</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D83" s="4"/>
-      <c r="E83" s="3"/>
-    </row>
-    <row r="84" spans="2:5" ht="18">
-      <c r="B84" s="1">
+      <c r="D83" s="3" t="n"/>
+      <c r="E83" s="4" t="n"/>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="B84" s="1" t="n">
         <v>81</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-    </row>
-    <row r="85" spans="2:5" ht="18">
-      <c r="B85" s="1">
+      <c r="D84" s="4" t="n"/>
+      <c r="E84" s="3" t="n"/>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="B85" s="1" t="n">
         <v>82</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-    </row>
-    <row r="86" spans="2:5" ht="18">
-      <c r="B86" s="1">
+      <c r="D85" s="4" t="n"/>
+      <c r="E85" s="4" t="n"/>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="B86" s="1" t="n">
         <v>83</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-    </row>
-    <row r="87" spans="2:5" ht="18">
-      <c r="B87" s="1">
+      <c r="D86" s="4" t="n"/>
+      <c r="E86" s="4" t="n"/>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="B87" s="1" t="n">
         <v>84</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
-    </row>
-    <row r="88" spans="2:5" ht="18">
-      <c r="B88" s="1">
+      <c r="D87" s="3" t="n"/>
+      <c r="E87" s="4" t="n"/>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="B88" s="1" t="n">
         <v>85</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
-    </row>
-    <row r="89" spans="2:5" ht="18">
-      <c r="B89" s="1">
+      <c r="D88" s="4" t="n"/>
+      <c r="E88" s="3" t="n"/>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="B89" s="1" t="n">
         <v>86</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D89" s="3"/>
-      <c r="E89" s="4"/>
-    </row>
-    <row r="90" spans="2:5" ht="18">
-      <c r="B90" s="1">
+      <c r="D89" s="4" t="n"/>
+      <c r="E89" s="4" t="n"/>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="B90" s="1" t="n">
         <v>87</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
-    </row>
-    <row r="91" spans="2:5" ht="18">
-      <c r="B91" s="1">
+      <c r="D90" s="3" t="n"/>
+      <c r="E90" s="3" t="n"/>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="B91" s="1" t="n">
         <v>88</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D91" s="3"/>
-      <c r="E91" s="4"/>
-    </row>
-    <row r="92" spans="2:5" ht="18">
-      <c r="B92" s="1">
+      <c r="D91" s="3" t="n"/>
+      <c r="E91" s="3" t="n"/>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="B92" s="1" t="n">
         <v>89</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D92" s="3"/>
-      <c r="E92" s="4"/>
-    </row>
-    <row r="93" spans="2:5" ht="18">
-      <c r="B93" s="1">
+      <c r="D92" s="3" t="n"/>
+      <c r="E92" s="3" t="n"/>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="B93" s="1" t="n">
         <v>90</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D93" s="3"/>
-      <c r="E93" s="4"/>
-    </row>
-    <row r="94" spans="2:5" ht="18">
-      <c r="B94" s="1">
+      <c r="D93" s="3" t="n"/>
+      <c r="E93" s="4" t="n"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="B94" s="1" t="n">
         <v>91</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D94" s="4"/>
-      <c r="E94" s="3"/>
-    </row>
-    <row r="95" spans="2:5" ht="18">
-      <c r="B95" s="1">
+      <c r="D94" s="3" t="n"/>
+      <c r="E94" s="4" t="n"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="B95" s="1" t="n">
         <v>92</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D95" s="4"/>
-      <c r="E95" s="4"/>
-    </row>
-    <row r="96" spans="2:5" ht="18">
-      <c r="B96" s="1">
+      <c r="D95" s="4" t="n"/>
+      <c r="E95" s="4" t="n"/>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="B96" s="1" t="n">
         <v>93</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D96" s="4"/>
-      <c r="E96" s="4"/>
-    </row>
-    <row r="97" spans="2:5" ht="18">
-      <c r="B97" s="1">
+      <c r="D96" s="4" t="n"/>
+      <c r="E96" s="3" t="n"/>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="B97" s="1" t="n">
         <v>94</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D97" s="4"/>
-      <c r="E97" s="4"/>
-    </row>
-    <row r="98" spans="2:5" ht="18">
-      <c r="B98" s="1">
+      <c r="D97" s="3" t="n"/>
+      <c r="E97" s="4" t="n"/>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="B98" s="1" t="n">
         <v>95</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D98" s="4"/>
-      <c r="E98" s="4"/>
-    </row>
-    <row r="99" spans="2:5" ht="18">
-      <c r="B99" s="1">
+      <c r="D98" s="4" t="n"/>
+      <c r="E98" s="4" t="n"/>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="B99" s="1" t="n">
         <v>96</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D99" s="4"/>
-      <c r="E99" s="3"/>
-    </row>
-    <row r="100" spans="2:5" ht="18">
-      <c r="B100" s="1">
+      <c r="D99" s="4" t="n"/>
+      <c r="E99" s="4" t="n"/>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="B100" s="1" t="n">
         <v>97</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D100" s="4"/>
-      <c r="E100" s="4"/>
-    </row>
-    <row r="101" spans="2:5" ht="18">
-      <c r="B101" s="1">
+      <c r="D100" s="4" t="n"/>
+      <c r="E100" s="4" t="n"/>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="B101" s="1" t="n">
         <v>98</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D101" s="3"/>
-      <c r="E101" s="4"/>
-    </row>
-    <row r="102" spans="2:5" ht="18">
-      <c r="B102" s="1">
+      <c r="D101" s="4" t="n"/>
+      <c r="E101" s="4" t="n"/>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="B102" s="1" t="n">
         <v>99</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D102" s="4"/>
-      <c r="E102" s="3"/>
-    </row>
-    <row r="103" spans="2:5" ht="18">
-      <c r="B103" s="1">
+      <c r="D102" s="4" t="n"/>
+      <c r="E102" s="3" t="n"/>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="B103" s="1" t="n">
         <v>100</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D103" s="4"/>
-      <c r="E103" s="4"/>
-    </row>
-    <row r="104" spans="2:5" ht="18">
-      <c r="B104" s="1">
+      <c r="D103" s="4" t="n"/>
+      <c r="E103" s="4" t="n"/>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="B104" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D104" s="4"/>
-      <c r="E104" s="4"/>
-    </row>
-    <row r="105" spans="2:5" ht="18">
-      <c r="B105" s="1">
+      <c r="D104" s="4" t="n"/>
+      <c r="E104" s="4" t="n"/>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="B105" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D105" s="4"/>
-      <c r="E105" s="3"/>
-    </row>
-    <row r="106" spans="2:5" ht="18">
-      <c r="B106" s="1">
+      <c r="D105" s="4" t="n"/>
+      <c r="E105" s="3" t="n"/>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="B106" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D106" s="4"/>
-      <c r="E106" s="4"/>
-    </row>
-    <row r="107" spans="2:5" ht="18">
-      <c r="B107" s="1">
+      <c r="D106" s="4" t="n"/>
+      <c r="E106" s="4" t="n"/>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="B107" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D107" s="4"/>
-      <c r="E107" s="4"/>
-    </row>
-    <row r="108" spans="2:5" ht="18">
-      <c r="B108" s="1">
+      <c r="D107" s="4" t="n"/>
+      <c r="E107" s="4" t="n"/>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="B108" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D108" s="3"/>
-      <c r="E108" s="4"/>
-    </row>
-    <row r="109" spans="2:5" ht="18">
-      <c r="B109" s="1">
+      <c r="D108" s="4" t="n"/>
+      <c r="E108" s="3" t="n"/>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="B109" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D109" s="3"/>
-      <c r="E109" s="3"/>
-    </row>
-    <row r="110" spans="2:5" ht="18">
-      <c r="B110" s="1">
+      <c r="D109" s="4" t="n"/>
+      <c r="E109" s="4" t="n"/>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="B110" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D110" s="3"/>
-      <c r="E110" s="4"/>
-    </row>
-    <row r="111" spans="2:5" ht="18">
-      <c r="B111" s="1">
+      <c r="D110" s="4" t="n"/>
+      <c r="E110" s="4" t="n"/>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="B111" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D111" s="3"/>
-      <c r="E111" s="4"/>
-    </row>
-    <row r="112" spans="2:5" ht="18">
-      <c r="B112" s="1">
+      <c r="D111" s="3" t="n"/>
+      <c r="E111" s="4" t="n"/>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="B112" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D112" s="3"/>
-      <c r="E112" s="4"/>
-    </row>
-    <row r="113" spans="2:5" ht="18">
-      <c r="B113" s="1">
+      <c r="D112" s="3" t="n"/>
+      <c r="E112" s="4" t="n"/>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="B113" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D113" s="3"/>
-      <c r="E113" s="4"/>
-    </row>
-    <row r="114" spans="2:5" ht="18">
-      <c r="B114" s="1">
+      <c r="D113" s="3" t="n"/>
+      <c r="E113" s="4" t="n"/>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="B114" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D114" s="3"/>
-      <c r="E114" s="4"/>
-    </row>
-    <row r="115" spans="2:5" ht="18">
-      <c r="B115" s="1">
+      <c r="D114" s="3" t="n"/>
+      <c r="E114" s="4" t="n"/>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="B115" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D115" s="3"/>
-      <c r="E115" s="4"/>
-    </row>
-    <row r="116" spans="2:5" ht="18">
-      <c r="B116" s="1">
+      <c r="D115" s="3" t="n"/>
+      <c r="E115" s="4" t="n"/>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="B116" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D116" s="3"/>
-      <c r="E116" s="4"/>
-    </row>
-    <row r="117" spans="2:5" ht="18">
-      <c r="B117" s="1">
+      <c r="D116" s="3" t="n"/>
+      <c r="E116" s="4" t="n"/>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="B117" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D117" s="3"/>
-      <c r="E117" s="4"/>
-    </row>
-    <row r="118" spans="2:5" ht="18">
-      <c r="B118" s="1">
+      <c r="D117" s="3" t="n"/>
+      <c r="E117" s="4" t="n"/>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="B118" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D118" s="3"/>
-      <c r="E118" s="4"/>
-    </row>
-    <row r="119" spans="2:5" ht="18">
-      <c r="B119" s="1">
+      <c r="D118" s="3" t="n"/>
+      <c r="E118" s="4" t="n"/>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="B119" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D119" s="3"/>
-      <c r="E119" s="4"/>
-    </row>
-    <row r="120" spans="2:5" ht="18">
-      <c r="B120" s="1">
+      <c r="D119" s="3" t="n"/>
+      <c r="E119" s="4" t="n"/>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="B120" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D120" s="3"/>
-      <c r="E120" s="4"/>
-    </row>
-    <row r="121" spans="2:5" ht="18">
-      <c r="B121" s="1">
+      <c r="D120" s="3" t="n"/>
+      <c r="E120" s="4" t="n"/>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="B121" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D121" s="3"/>
-      <c r="E121" s="4"/>
-    </row>
-    <row r="122" spans="2:5" ht="18">
-      <c r="B122" s="1">
+      <c r="D121" s="3" t="n"/>
+      <c r="E121" s="4" t="n"/>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="B122" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D122" s="3"/>
-      <c r="E122" s="4"/>
-    </row>
-    <row r="123" spans="2:5" ht="18">
-      <c r="B123" s="1">
+      <c r="D122" s="3" t="n"/>
+      <c r="E122" s="4" t="n"/>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="B123" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D123" s="3"/>
-      <c r="E123" s="4"/>
-    </row>
-    <row r="124" spans="2:5" ht="18">
-      <c r="B124" s="1">
+      <c r="D123" s="3" t="n"/>
+      <c r="E123" s="4" t="n"/>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="B124" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D124" s="3"/>
-      <c r="E124" s="4"/>
-    </row>
-    <row r="125" spans="2:5" ht="18">
-      <c r="B125" s="1">
+      <c r="D124" s="3" t="n"/>
+      <c r="E124" s="4" t="n"/>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="B125" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D125" s="3"/>
-      <c r="E125" s="4"/>
-    </row>
-    <row r="126" spans="2:5" ht="18">
-      <c r="B126" s="1">
+      <c r="D125" s="3" t="n"/>
+      <c r="E125" s="4" t="n"/>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="B126" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D126" s="3"/>
-      <c r="E126" s="4"/>
-    </row>
-    <row r="127" spans="2:5" ht="18">
-      <c r="B127" s="1">
+      <c r="D126" s="3" t="n"/>
+      <c r="E126" s="4" t="n"/>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="B127" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D127" s="3"/>
-      <c r="E127" s="4"/>
-    </row>
-    <row r="128" spans="2:5" ht="18">
-      <c r="B128" s="1">
+      <c r="D127" s="3" t="n"/>
+      <c r="E127" s="4" t="n"/>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="B128" s="1" t="n">
         <v>101</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D128" s="4"/>
-      <c r="E128" s="3"/>
-    </row>
-    <row r="129" spans="2:5">
-      <c r="B129" s="10">
-        <v>101</v>
-      </c>
-      <c r="C129" s="10" t="s">
+      <c r="D128" s="3" t="n"/>
+      <c r="E128" s="4" t="n"/>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="B129" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C129" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D129" s="4"/>
-      <c r="E129" s="3"/>
-    </row>
-    <row r="130" spans="2:5">
-      <c r="B130" s="10">
-        <v>101</v>
-      </c>
-      <c r="C130" s="10" t="s">
+      <c r="D129" s="3" t="n"/>
+      <c r="E129" s="4" t="n"/>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="B130" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D130" s="4"/>
-      <c r="E130" s="3"/>
-    </row>
-    <row r="131" spans="2:5">
-      <c r="B131" s="10">
-        <v>101</v>
-      </c>
-      <c r="C131" s="10" t="s">
+      <c r="D130" s="4" t="n"/>
+      <c r="E130" s="3" t="n"/>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="B131" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C131" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D131" s="4"/>
-      <c r="E131" s="3"/>
+      <c r="D131" s="4" t="n"/>
+      <c r="E131" s="3" t="n"/>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="B132" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D132" s="4" t="n"/>
+      <c r="E132" s="3" t="n"/>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="B133" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D133" s="4" t="n"/>
+      <c r="E133" s="3" t="n"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated requirements to safe requests version. Add some xls files.
</commit_message>
<xml_diff>
--- a/OWGR.xlsx
+++ b/OWGR.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="135">
   <si>
     <t>RANK</t>
   </si>
@@ -32,12 +32,12 @@
     <t>Johnson, Dustin</t>
   </si>
   <si>
+    <t>Thomas, Justin</t>
+  </si>
+  <si>
     <t>Rahm, Jon</t>
   </si>
   <si>
-    <t>Thomas, Justin</t>
-  </si>
-  <si>
     <t>Spieth, Jordan</t>
   </si>
   <si>
@@ -50,19 +50,22 @@
     <t>Fowler, Rickie</t>
   </si>
   <si>
+    <t>Koepka, Brooks</t>
+  </si>
+  <si>
     <t>Day, Jason</t>
   </si>
   <si>
-    <t>Koepka, Brooks</t>
+    <t>Fleetwood, Tommy</t>
+  </si>
+  <si>
+    <t>Garcia, Sergio</t>
   </si>
   <si>
     <t>McIlroy, Rory</t>
   </si>
   <si>
-    <t>Fleetwood, Tommy</t>
-  </si>
-  <si>
-    <t>Garcia, Sergio</t>
+    <t>Hatton, Tyrrell</t>
   </si>
   <si>
     <t>Stenson, Henrik</t>
@@ -74,30 +77,30 @@
     <t>Leishman, Marc</t>
   </si>
   <si>
-    <t>Hatton, Tyrrell</t>
-  </si>
-  <si>
     <t>Casey, Paul</t>
   </si>
   <si>
+    <t>Mickelson, Phil</t>
+  </si>
+  <si>
+    <t>Perez, Pat</t>
+  </si>
+  <si>
     <t>Kuchar, Matt</t>
   </si>
   <si>
-    <t>Perez, Pat</t>
-  </si>
-  <si>
     <t>Cabrera Bello, Rafael</t>
   </si>
   <si>
     <t>Harman, Brian</t>
   </si>
   <si>
+    <t>Schauffele, Xander</t>
+  </si>
+  <si>
     <t>Molinari, Francesco</t>
   </si>
   <si>
-    <t>Schauffele, Xander</t>
-  </si>
-  <si>
     <t>Hoffman, Charley</t>
   </si>
   <si>
@@ -107,15 +110,18 @@
     <t>Reed, Patrick</t>
   </si>
   <si>
+    <t>Grace, Branden</t>
+  </si>
+  <si>
     <t>Fisher, Ross</t>
   </si>
   <si>
-    <t>Grace, Branden</t>
-  </si>
-  <si>
     <t>Oosthuizen, Louis</t>
   </si>
   <si>
+    <t>Berger, Daniel</t>
+  </si>
+  <si>
     <t>Fitzpatrick, Matthew</t>
   </si>
   <si>
@@ -125,39 +131,36 @@
     <t>Finau, Tony</t>
   </si>
   <si>
-    <t>Berger, Daniel</t>
-  </si>
-  <si>
-    <t>Mickelson, Phil</t>
-  </si>
-  <si>
     <t>Cantlay, Patrick</t>
   </si>
   <si>
+    <t>Aphibarnrat, Kiradech</t>
+  </si>
+  <si>
     <t>Chappell, Kevin</t>
   </si>
   <si>
+    <t>Watson, Bubba</t>
+  </si>
+  <si>
+    <t>Steele, Brendan</t>
+  </si>
+  <si>
     <t>Haotong, Li</t>
   </si>
   <si>
-    <t>Steele, Brendan</t>
-  </si>
-  <si>
     <t>Pieters, Thomas</t>
   </si>
   <si>
-    <t>Aphibarnrat, Kiradech</t>
-  </si>
-  <si>
     <t>Simpson, Webb</t>
   </si>
   <si>
-    <t>Watson, Bubba</t>
-  </si>
-  <si>
     <t>Kodaira, Satoshi</t>
   </si>
   <si>
+    <t>Hadwin, Adam</t>
+  </si>
+  <si>
     <t>Frittelli, Dylan</t>
   </si>
   <si>
@@ -167,48 +170,45 @@
     <t>Reavie, Chez</t>
   </si>
   <si>
+    <t>Vegas, Jhonattan</t>
+  </si>
+  <si>
+    <t>Ikeda, Yuta</t>
+  </si>
+  <si>
     <t>Schwartzel, Charl</t>
   </si>
   <si>
-    <t>Ikeda, Yuta</t>
-  </si>
-  <si>
-    <t>Hadwin, Adam</t>
-  </si>
-  <si>
-    <t>Vegas, Jhonattan</t>
+    <t>Kizzire, Patton</t>
+  </si>
+  <si>
+    <t>Smith, Cameron</t>
   </si>
   <si>
     <t>Kim, Siwoo</t>
   </si>
   <si>
-    <t>Smith, Cameron</t>
-  </si>
-  <si>
     <t>Wiesberger, Bernd</t>
   </si>
   <si>
+    <t>Stanley, Kyle</t>
+  </si>
+  <si>
+    <t>Henley, Russell</t>
+  </si>
+  <si>
     <t>Miyazato, Yusaku</t>
   </si>
   <si>
-    <t>Henley, Russell</t>
-  </si>
-  <si>
     <t>Scott, Adam</t>
   </si>
   <si>
-    <t>Stanley, Kyle</t>
+    <t>Johnson, Zach</t>
   </si>
   <si>
     <t>Hahn, James</t>
   </si>
   <si>
-    <t>Kizzire, Patton</t>
-  </si>
-  <si>
-    <t>Johnson, Zach</t>
-  </si>
-  <si>
     <t>Levy, Alexander</t>
   </si>
   <si>
@@ -224,106 +224,109 @@
     <t>Na, Kevin</t>
   </si>
   <si>
+    <t>Sharma, Shubhankar</t>
+  </si>
+  <si>
+    <t>Luiten, Joost</t>
+  </si>
+  <si>
     <t>Moore, Ryan</t>
   </si>
   <si>
-    <t>Luiten, Joost</t>
-  </si>
-  <si>
     <t>Bradley, Keegan</t>
   </si>
   <si>
+    <t>Suri, Julian</t>
+  </si>
+  <si>
     <t>Haas, Bill</t>
   </si>
   <si>
-    <t>Suri, Julian</t>
-  </si>
-  <si>
     <t>Hadley, Chesson</t>
   </si>
   <si>
+    <t>List, Luke</t>
+  </si>
+  <si>
     <t>Snedeker, Brandt</t>
   </si>
   <si>
-    <t>List, Luke</t>
-  </si>
-  <si>
     <t>Lowry, Shane</t>
   </si>
   <si>
-    <t>Sharma, Shubhankar</t>
-  </si>
-  <si>
     <t>Grillo, Emiliano</t>
   </si>
   <si>
+    <t>Potter Jr, Ted</t>
+  </si>
+  <si>
+    <t>Paisley, Chris</t>
+  </si>
+  <si>
     <t>Tanihara, Hideto</t>
   </si>
   <si>
-    <t>Potter Jr, Ted</t>
-  </si>
-  <si>
     <t>Lahiri, Anirban</t>
   </si>
   <si>
+    <t>Dunne, Paul</t>
+  </si>
+  <si>
+    <t>Horschel, Billy</t>
+  </si>
+  <si>
+    <t>Schniederjans, Ollie</t>
+  </si>
+  <si>
     <t>Westwood, Lee</t>
   </si>
   <si>
-    <t>Schniederjans, Ollie</t>
-  </si>
-  <si>
     <t>Han, Seungsu</t>
   </si>
   <si>
-    <t>Paisley, Chris</t>
-  </si>
-  <si>
     <t>Hun An, Byeong</t>
   </si>
   <si>
     <t>Bryan, Wesley</t>
   </si>
   <si>
-    <t>Dunne, Paul</t>
-  </si>
-  <si>
-    <t>Horschel, Billy</t>
-  </si>
-  <si>
     <t>Kaymer, Martin</t>
   </si>
   <si>
     <t>Walker, Jimmy</t>
   </si>
   <si>
+    <t>Wood, Chris</t>
+  </si>
+  <si>
     <t>Holmes, J.B.</t>
   </si>
   <si>
-    <t>Wood, Chris</t>
-  </si>
-  <si>
     <t>Pepperell, Eddie</t>
   </si>
   <si>
     <t>Kang, Sunghoon</t>
   </si>
   <si>
+    <t>DeChambeau, Bryson</t>
+  </si>
+  <si>
+    <t>Glover, Lucas</t>
+  </si>
+  <si>
+    <t>Olesen, Thorbjorn</t>
+  </si>
+  <si>
+    <t>Kim, Chan</t>
+  </si>
+  <si>
     <t>Knox, Russell</t>
   </si>
   <si>
-    <t>DeChambeau, Bryson</t>
-  </si>
-  <si>
-    <t>Olesen, Thorbjorn</t>
-  </si>
-  <si>
-    <t>Kim, Chan</t>
+    <t>Coetzee, George</t>
   </si>
   <si>
     <t>Lovemark, Jamie</t>
-  </si>
-  <si>
-    <t>Glover, Lucas</t>
   </si>
   <si>
     <t>Zanotti, Fabrizio</t>
@@ -511,8 +514,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table1" headerRowCount="1" id="1" name="Table1" ref="B3:E133">
-  <autoFilter ref="B3:E133"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table1" headerRowCount="1" id="1" name="Table1" ref="B3:E134">
+  <autoFilter ref="B3:E134"/>
   <tableColumns count="4">
     <tableColumn id="2" name="RANK"/>
     <tableColumn id="3" name="Player Name"/>
@@ -812,7 +815,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:F133"/>
+  <dimension ref="A3:F134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -948,7 +951,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="3" t="n"/>
-      <c r="E14" s="4" t="n"/>
+      <c r="E14" s="3" t="n"/>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="1" t="n">
@@ -958,7 +961,7 @@
         <v>15</v>
       </c>
       <c r="D15" s="3" t="n"/>
-      <c r="E15" s="3" t="n"/>
+      <c r="E15" s="4" t="n"/>
     </row>
     <row r="16" spans="1:6">
       <c r="B16" s="1" t="n">
@@ -967,8 +970,8 @@
       <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="3" t="n"/>
-      <c r="E16" s="4" t="n"/>
+      <c r="D16" s="4" t="n"/>
+      <c r="E16" s="3" t="n"/>
     </row>
     <row r="17" spans="1:6">
       <c r="B17" s="1" t="n">
@@ -978,7 +981,7 @@
         <v>17</v>
       </c>
       <c r="D17" s="3" t="n"/>
-      <c r="E17" s="3" t="n"/>
+      <c r="E17" s="4" t="n"/>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" s="1" t="n">
@@ -988,7 +991,7 @@
         <v>18</v>
       </c>
       <c r="D18" s="3" t="n"/>
-      <c r="E18" s="4" t="n"/>
+      <c r="E18" s="3" t="n"/>
     </row>
     <row r="19" spans="1:6">
       <c r="B19" s="1" t="n">
@@ -997,8 +1000,8 @@
       <c r="C19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="4" t="n"/>
-      <c r="E19" s="3" t="n"/>
+      <c r="D19" s="3" t="n"/>
+      <c r="E19" s="4" t="n"/>
     </row>
     <row r="20" spans="1:6">
       <c r="B20" s="1" t="n">
@@ -1038,7 +1041,7 @@
         <v>23</v>
       </c>
       <c r="D23" s="3" t="n"/>
-      <c r="E23" s="3" t="n"/>
+      <c r="E23" s="4" t="n"/>
     </row>
     <row r="24" spans="1:6">
       <c r="B24" s="1" t="n">
@@ -1047,8 +1050,8 @@
       <c r="C24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="4" t="n"/>
-      <c r="E24" s="4" t="n"/>
+      <c r="D24" s="3" t="n"/>
+      <c r="E24" s="3" t="n"/>
     </row>
     <row r="25" spans="1:6">
       <c r="B25" s="1" t="n">
@@ -1057,7 +1060,7 @@
       <c r="C25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="3" t="n"/>
+      <c r="D25" s="4" t="n"/>
       <c r="E25" s="4" t="n"/>
     </row>
     <row r="26" spans="1:6">
@@ -1077,7 +1080,7 @@
       <c r="C27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="4" t="n"/>
+      <c r="D27" s="3" t="n"/>
       <c r="E27" s="4" t="n"/>
     </row>
     <row r="28" spans="1:6">
@@ -1087,8 +1090,8 @@
       <c r="C28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="3" t="n"/>
-      <c r="E28" s="3" t="n"/>
+      <c r="D28" s="4" t="n"/>
+      <c r="E28" s="4" t="n"/>
     </row>
     <row r="29" spans="1:6">
       <c r="B29" s="1" t="n">
@@ -1098,7 +1101,7 @@
         <v>29</v>
       </c>
       <c r="D29" s="3" t="n"/>
-      <c r="E29" s="4" t="n"/>
+      <c r="E29" s="3" t="n"/>
     </row>
     <row r="30" spans="1:6">
       <c r="B30" s="1" t="n">
@@ -1128,7 +1131,7 @@
         <v>32</v>
       </c>
       <c r="D32" s="3" t="n"/>
-      <c r="E32" s="3" t="n"/>
+      <c r="E32" s="4" t="n"/>
     </row>
     <row r="33" spans="1:6">
       <c r="B33" s="1" t="n">
@@ -1137,8 +1140,8 @@
       <c r="C33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="4" t="n"/>
-      <c r="E33" s="4" t="n"/>
+      <c r="D33" s="3" t="n"/>
+      <c r="E33" s="3" t="n"/>
     </row>
     <row r="34" spans="1:6">
       <c r="B34" s="1" t="n">
@@ -1177,7 +1180,7 @@
       <c r="C37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="3" t="n"/>
+      <c r="D37" s="4" t="n"/>
       <c r="E37" s="4" t="n"/>
     </row>
     <row r="38" spans="1:6">
@@ -1197,7 +1200,7 @@
       <c r="C39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="3" t="n"/>
+      <c r="D39" s="4" t="n"/>
       <c r="E39" s="4" t="n"/>
     </row>
     <row r="40" spans="1:6">
@@ -1207,7 +1210,7 @@
       <c r="C40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="4" t="n"/>
+      <c r="D40" s="3" t="n"/>
       <c r="E40" s="4" t="n"/>
     </row>
     <row r="41" spans="1:6">
@@ -1248,17 +1251,17 @@
         <v>44</v>
       </c>
       <c r="D44" s="3" t="n"/>
-      <c r="E44" s="3" t="n"/>
+      <c r="E44" s="4" t="n"/>
     </row>
     <row r="45" spans="1:6">
       <c r="B45" s="1" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D45" s="3" t="n"/>
-      <c r="E45" s="4" t="n"/>
+      <c r="E45" s="3" t="n"/>
     </row>
     <row r="46" spans="1:6">
       <c r="B46" s="1" t="n">
@@ -1277,7 +1280,7 @@
       <c r="C47" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="4" t="n"/>
+      <c r="D47" s="3" t="n"/>
       <c r="E47" s="4" t="n"/>
     </row>
     <row r="48" spans="1:6">
@@ -1287,7 +1290,7 @@
       <c r="C48" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D48" s="3" t="n"/>
+      <c r="D48" s="4" t="n"/>
       <c r="E48" s="4" t="n"/>
     </row>
     <row r="49" spans="1:6">
@@ -1297,7 +1300,7 @@
       <c r="C49" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D49" s="4" t="n"/>
+      <c r="D49" s="3" t="n"/>
       <c r="E49" s="4" t="n"/>
     </row>
     <row r="50" spans="1:6">
@@ -1307,7 +1310,7 @@
       <c r="C50" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="3" t="n"/>
+      <c r="D50" s="4" t="n"/>
       <c r="E50" s="4" t="n"/>
     </row>
     <row r="51" spans="1:6">
@@ -1348,7 +1351,7 @@
         <v>54</v>
       </c>
       <c r="D54" s="4" t="n"/>
-      <c r="E54" s="4" t="n"/>
+      <c r="E54" s="3" t="n"/>
     </row>
     <row r="55" spans="1:6">
       <c r="B55" s="1" t="n">
@@ -1367,7 +1370,7 @@
       <c r="C56" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D56" s="3" t="n"/>
+      <c r="D56" s="4" t="n"/>
       <c r="E56" s="4" t="n"/>
     </row>
     <row r="57" spans="1:6">
@@ -1377,7 +1380,7 @@
       <c r="C57" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D57" s="4" t="n"/>
+      <c r="D57" s="3" t="n"/>
       <c r="E57" s="4" t="n"/>
     </row>
     <row r="58" spans="1:6">
@@ -1388,7 +1391,7 @@
         <v>58</v>
       </c>
       <c r="D58" s="4" t="n"/>
-      <c r="E58" s="3" t="n"/>
+      <c r="E58" s="4" t="n"/>
     </row>
     <row r="59" spans="1:6">
       <c r="B59" s="1" t="n">
@@ -1398,7 +1401,7 @@
         <v>59</v>
       </c>
       <c r="D59" s="4" t="n"/>
-      <c r="E59" s="4" t="n"/>
+      <c r="E59" s="3" t="n"/>
     </row>
     <row r="60" spans="1:6">
       <c r="B60" s="1" t="n">
@@ -1427,8 +1430,8 @@
       <c r="C62" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D62" s="4" t="n"/>
-      <c r="E62" s="3" t="n"/>
+      <c r="D62" s="3" t="n"/>
+      <c r="E62" s="4" t="n"/>
     </row>
     <row r="63" spans="1:6">
       <c r="B63" s="1" t="n">
@@ -1437,7 +1440,7 @@
       <c r="C63" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D63" s="3" t="n"/>
+      <c r="D63" s="4" t="n"/>
       <c r="E63" s="4" t="n"/>
     </row>
     <row r="64" spans="1:6">
@@ -1499,7 +1502,7 @@
       <c r="C69" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D69" s="3" t="n"/>
+      <c r="D69" s="4" t="n"/>
       <c r="E69" s="4" t="n"/>
     </row>
     <row r="70" spans="1:6">
@@ -1519,7 +1522,7 @@
       <c r="C71" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D71" s="4" t="n"/>
+      <c r="D71" s="3" t="n"/>
       <c r="E71" s="4" t="n"/>
     </row>
     <row r="72" spans="1:6">
@@ -1529,7 +1532,7 @@
       <c r="C72" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D72" s="3" t="n"/>
+      <c r="D72" s="4" t="n"/>
       <c r="E72" s="4" t="n"/>
     </row>
     <row r="73" spans="1:6">
@@ -1549,8 +1552,8 @@
       <c r="C74" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D74" s="4" t="n"/>
-      <c r="E74" s="3" t="n"/>
+      <c r="D74" s="3" t="n"/>
+      <c r="E74" s="4" t="n"/>
     </row>
     <row r="75" spans="1:6">
       <c r="B75" s="1" t="n">
@@ -1559,7 +1562,7 @@
       <c r="C75" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D75" s="3" t="n"/>
+      <c r="D75" s="4" t="n"/>
       <c r="E75" s="3" t="n"/>
     </row>
     <row r="76" spans="1:6">
@@ -1589,8 +1592,8 @@
       <c r="C78" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D78" s="4" t="n"/>
-      <c r="E78" s="4" t="n"/>
+      <c r="D78" s="3" t="n"/>
+      <c r="E78" s="3" t="n"/>
     </row>
     <row r="79" spans="1:6">
       <c r="B79" s="1" t="n">
@@ -1609,8 +1612,8 @@
       <c r="C80" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D80" s="3" t="n"/>
-      <c r="E80" s="4" t="n"/>
+      <c r="D80" s="4" t="n"/>
+      <c r="E80" s="3" t="n"/>
     </row>
     <row r="81" spans="1:6">
       <c r="B81" s="1" t="n">
@@ -1620,7 +1623,7 @@
         <v>81</v>
       </c>
       <c r="D81" s="4" t="n"/>
-      <c r="E81" s="3" t="n"/>
+      <c r="E81" s="4" t="n"/>
     </row>
     <row r="82" spans="1:6">
       <c r="B82" s="1" t="n">
@@ -1629,7 +1632,7 @@
       <c r="C82" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D82" s="4" t="n"/>
+      <c r="D82" s="3" t="n"/>
       <c r="E82" s="4" t="n"/>
     </row>
     <row r="83" spans="1:6">
@@ -1639,7 +1642,7 @@
       <c r="C83" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D83" s="3" t="n"/>
+      <c r="D83" s="4" t="n"/>
       <c r="E83" s="4" t="n"/>
     </row>
     <row r="84" spans="1:6">
@@ -1650,7 +1653,7 @@
         <v>84</v>
       </c>
       <c r="D84" s="4" t="n"/>
-      <c r="E84" s="3" t="n"/>
+      <c r="E84" s="4" t="n"/>
     </row>
     <row r="85" spans="1:6">
       <c r="B85" s="1" t="n">
@@ -1659,8 +1662,8 @@
       <c r="C85" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D85" s="4" t="n"/>
-      <c r="E85" s="4" t="n"/>
+      <c r="D85" s="3" t="n"/>
+      <c r="E85" s="3" t="n"/>
     </row>
     <row r="86" spans="1:6">
       <c r="B86" s="1" t="n">
@@ -1670,7 +1673,7 @@
         <v>86</v>
       </c>
       <c r="D86" s="4" t="n"/>
-      <c r="E86" s="4" t="n"/>
+      <c r="E86" s="3" t="n"/>
     </row>
     <row r="87" spans="1:6">
       <c r="B87" s="1" t="n">
@@ -1690,7 +1693,7 @@
         <v>88</v>
       </c>
       <c r="D88" s="4" t="n"/>
-      <c r="E88" s="3" t="n"/>
+      <c r="E88" s="4" t="n"/>
     </row>
     <row r="89" spans="1:6">
       <c r="B89" s="1" t="n">
@@ -1699,7 +1702,7 @@
       <c r="C89" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D89" s="4" t="n"/>
+      <c r="D89" s="3" t="n"/>
       <c r="E89" s="4" t="n"/>
     </row>
     <row r="90" spans="1:6">
@@ -1709,7 +1712,7 @@
       <c r="C90" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D90" s="3" t="n"/>
+      <c r="D90" s="4" t="n"/>
       <c r="E90" s="3" t="n"/>
     </row>
     <row r="91" spans="1:6">
@@ -1779,7 +1782,7 @@
       <c r="C97" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D97" s="3" t="n"/>
+      <c r="D97" s="4" t="n"/>
       <c r="E97" s="4" t="n"/>
     </row>
     <row r="98" spans="1:6">
@@ -1790,7 +1793,7 @@
         <v>98</v>
       </c>
       <c r="D98" s="4" t="n"/>
-      <c r="E98" s="4" t="n"/>
+      <c r="E98" s="3" t="n"/>
     </row>
     <row r="99" spans="1:6">
       <c r="B99" s="1" t="n">
@@ -1804,7 +1807,7 @@
     </row>
     <row r="100" spans="1:6">
       <c r="B100" s="1" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>100</v>
@@ -1819,7 +1822,7 @@
       <c r="C101" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D101" s="4" t="n"/>
+      <c r="D101" s="3" t="n"/>
       <c r="E101" s="4" t="n"/>
     </row>
     <row r="102" spans="1:6">
@@ -1830,7 +1833,7 @@
         <v>102</v>
       </c>
       <c r="D102" s="4" t="n"/>
-      <c r="E102" s="3" t="n"/>
+      <c r="E102" s="4" t="n"/>
     </row>
     <row r="103" spans="1:6">
       <c r="B103" s="1" t="n">
@@ -1860,7 +1863,7 @@
         <v>105</v>
       </c>
       <c r="D105" s="4" t="n"/>
-      <c r="E105" s="3" t="n"/>
+      <c r="E105" s="4" t="n"/>
     </row>
     <row r="106" spans="1:6">
       <c r="B106" s="1" t="n">
@@ -1870,7 +1873,7 @@
         <v>106</v>
       </c>
       <c r="D106" s="4" t="n"/>
-      <c r="E106" s="4" t="n"/>
+      <c r="E106" s="3" t="n"/>
     </row>
     <row r="107" spans="1:6">
       <c r="B107" s="1" t="n">
@@ -1890,7 +1893,7 @@
         <v>108</v>
       </c>
       <c r="D108" s="4" t="n"/>
-      <c r="E108" s="3" t="n"/>
+      <c r="E108" s="4" t="n"/>
     </row>
     <row r="109" spans="1:6">
       <c r="B109" s="1" t="n">
@@ -1900,7 +1903,7 @@
         <v>109</v>
       </c>
       <c r="D109" s="4" t="n"/>
-      <c r="E109" s="4" t="n"/>
+      <c r="E109" s="3" t="n"/>
     </row>
     <row r="110" spans="1:6">
       <c r="B110" s="1" t="n">
@@ -1919,7 +1922,7 @@
       <c r="C111" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D111" s="3" t="n"/>
+      <c r="D111" s="4" t="n"/>
       <c r="E111" s="4" t="n"/>
     </row>
     <row r="112" spans="1:6">
@@ -2109,8 +2112,8 @@
       <c r="C130" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D130" s="4" t="n"/>
-      <c r="E130" s="3" t="n"/>
+      <c r="D130" s="3" t="n"/>
+      <c r="E130" s="4" t="n"/>
     </row>
     <row r="131" spans="1:6">
       <c r="B131" s="1" t="n">
@@ -2141,6 +2144,16 @@
       </c>
       <c r="D133" s="4" t="n"/>
       <c r="E133" s="3" t="n"/>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="B134" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D134" s="4" t="n"/>
+      <c r="E134" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>